<commit_message>
(fix): Removed some files.
</commit_message>
<xml_diff>
--- a/DawnNews.xlsx
+++ b/DawnNews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,88 +480,88 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English ...</t>
+          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909395</t>
+          <t>https://www.dawn.com/news/1868819</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">08-May-2025 </t>
+          <t xml:space="preserve">31-Oct-2024 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
+          <t xml:space="preserve"> The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle- </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lahore receives highest rainfall of last 30 years: Wasa - Pakistan ...</t>
+          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1845401</t>
+          <t>https://www.dawn.com/news/1868279</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">12-Jul-2024 </t>
+          <t xml:space="preserve">29-Oct-2024 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding </t>
+          <t xml:space="preserve"> Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - DAWN ...</t>
+          <t>Lahore receives highest rainfall of last 30 years: Wasa - Pakistan ...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868819</t>
+          <t>https://www.dawn.com/news/1845401</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t xml:space="preserve">12-Jul-2024 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle- </t>
+          <t xml:space="preserve"> While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - DAWN ...</t>
+          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English ...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868279</t>
+          <t>https://www.dawn.com/news/1909395</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">29-Oct-2024 </t>
+          <t xml:space="preserve">08-May-2025 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
         </is>
       </c>
     </row>
@@ -612,176 +612,1012 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1869574</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t xml:space="preserve">03-Nov-2024 </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lahore again becomes world's most polluted city with 394 AQI ...</t>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866749</t>
+          <t>https://www.dawn.com/news/1869475</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">22-Oct-2024 </t>
+          <t xml:space="preserve">03-Nov-2024 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lahore-based coworking startup Colabs raises $2m in pre Series A ...</t>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1867329</t>
+          <t>https://www.dawn.com/news/1865801</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">24-Oct-2024 </t>
+          <t xml:space="preserve">17-Oct-2024 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Triumphant Arshad Nadeem lands in Lahore to rousing welcome ...</t>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1851530</t>
+          <t>https://www.dawn.com/news/1868870</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">11-Aug-2024 </t>
+          <t xml:space="preserve">31-Oct-2024 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> After striking gold at the Paris Olympics, ace javelin thrower Arshad Nadeem landed at the Lahore airport in the small hours of Sunday morning to a rousing </t>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weather Alert: Cold Weather Increased Due To Drizzle In Lahore ...</t>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1883239</t>
+          <t>https://www.dawn.com/news/1865270</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">05-Jan-2025 </t>
+          <t xml:space="preserve">15-Oct-2024 </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Weather Alert: Cold Weather Increased Due To Drizzle In Lahore | Breaking News | Dawn News.</t>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lahore ATC issues non-bailable arrest warrant for KP CM over ...</t>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905891</t>
+          <t>https://www.dawn.com/news/1897926</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">22-Apr-2025 </t>
+          <t xml:space="preserve">15-Mar-2025 </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>British artist's artwork highlights air pollution in Lahore - Newspaper ...</t>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865223</t>
+          <t>https://www.dawn.com/news/1869475</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t xml:space="preserve">03-Nov-2024 </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: British artist Dryden Goodwin's acclaimed artwork, Breathe, is a part of the ongoing Lahore Biennale 03</t>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lahore woman 'gang-raped' in front of husband, child - Pakistan ...</t>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1848007</t>
+          <t>https://www.dawn.com/news/1865801</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">26-Jul-2024 </t>
+          <t xml:space="preserve">17-Oct-2024 </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> نیتن یاہو کا انجام کیا ہوگا؟ Dawn News English </t>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1869475</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">03-Nov-2024 </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865801</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1868870</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">31-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865270</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Oct-2024 </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897926</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">15-Mar-2025 </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
(feat): Fixing checkpoint errors.
</commit_message>
<xml_diff>
--- a/DawnNews.xlsx
+++ b/DawnNews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,799 +458,787 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos ...</t>
+          <t>Parking chaos deepens in Lahore as agencies pass the buck - Dawn</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1892744</t>
+          <t>https://www.dawn.com/news/1917362</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Mar-2025 </t>
+          <t>16-Jun-2025</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
+          <t>The city's civic authorities appear to have no workable solution for Lahore's worsening parking crisis, with plans for setback areas in front of buildings and</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lahore receives highest rainfall of last 30 years: Wasa - Pakistan ...</t>
+          <t>Over 3,800 vehicles of govt depts don't give a hoot to traffic laws in ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1845401</t>
+          <t>https://www.dawn.com/news/1913330</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">12-Jul-2024 </t>
+          <t>26-May-2025</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding </t>
+          <t>LAHORE: Over 3,800 official vehicles of the government departments being used by senior bureaucrats and police officers were found violating</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - DAWN ...</t>
+          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868819</t>
+          <t>https://www.dawn.com/news/1904992</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>18-Apr-2025</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle- </t>
+          <t>Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English ...</t>
+          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909395</t>
+          <t>https://www.dawn.com/news/1909625</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">08-May-2025 </t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
+          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - DAWN ...</t>
+          <t>Fast-food chain outlet attacked in Lahore's DHA - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868279</t>
+          <t>https://www.dawn.com/news/1903292</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">29-Oct-2024 </t>
+          <t>10-Apr-2025</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its </t>
+          <t>LAHORE: An outlet of a fast-food chain on Wednesday came under an attack in Defense Housing Authority (DHA) when scores of people pelted it</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Suspect held for allegedly raping college student in Lahore: police ...</t>
+          <t>Public anger grows at traffic jams during PSL teams movement in ...</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1864994</t>
+          <t>https://www.dawn.com/news/1907199</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">13-Oct-2024 </t>
+          <t>29-Apr-2025</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
+          <t>LAHORE: Motorists and motorcyclists have run out of patience and started blaring horns during the movement of cricket teams participating in</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lahore police probing claims about disinformation that sparked UK ...</t>
+          <t>Latest - DAWN.COM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1853208</t>
+          <t>https://www.dawn.com/latest-news</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">19-Aug-2024 </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Lahore Deputy Inspector General (Operations) Faisal Kamran told Dawn they were analysing the claims made by UK broadcaster ITV News and had </t>
-        </is>
-      </c>
+          <t>Reaffirms commitment to Pak-China friendship; meets with foreign ministers of Iran, Uzbekistan, other SCO member states. Published about 8 hours ago</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+          <t>Lahore police use water cannons to disperse young doctors - Dawn</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869475</t>
+          <t>https://www.dawn.com/news/1905123</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>19-Apr-2025</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000 </t>
+          <t>LAHORE: The police used water cannons to disperse the protesting young doctors on the Mall Road, leaving two of the protesters,</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Two more bodies of Libya boat tragedy victims arrive in Lahore - Dawn</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1908386</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>04-May-2025</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>Two more bodies of Pakistan nationals who lost their lives in a tragic boat accident off the eastern coast of Libya, arrived at Lahore Airport on Sunday.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1892744</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>17-Mar-2025</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1887735</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>26-Jan-2025</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Lahore High Court summons AGP in pleas against X ban - Dawn</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1902909</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>08-Apr-2025</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>The Lahore High Court (LHC) on Tuesday summoned the Attorney General of Pakistan (AGP) Mansoor Usman Awan in a case pertaining to the ban on the social media</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>People in Lahore celebrate Pakistan Army's victory over India - Dawn</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1910253</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>11-May-2025</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>LAHORE: People burst into celebrations after the armed forces early on Saturday responded to Indian war hysteria in a befitting manner and</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1909395</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>08-May-2025</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Lahore High Court summons AGP in pleas against X ban - Dawn</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1902909</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>08-Apr-2025</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>The Lahore High Court (LHC) on Tuesday summoned the Attorney General of Pakistan (AGP) Mansoor Usman Awan in a case pertaining to the ban on the social media</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Lahore in the grip of a serious crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1870383</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>On the Air Quality Index (AQI), Lahore has been consistently registering hazardous levels, surpassing major metropolitan cities, like New Delhi</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1870214</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>PTI moves LHC to seek permission for Lahore rally - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1889622</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>04-Feb-2025</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>The Pakistan Tehreek-i-Insaf on Monday approached the Lahore High Court, seeking permission to hold a public rally at the Minar-i-Pakistan on Feb 8.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Lahore needs to do what London did - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1873583</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>20-Nov-2024</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>THERE are severe threats to human health and environment that smog poses to Lahore and other cities in Punjab. Every</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Govt shuts primary schools in Lahore over record pollution - Dawn</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1869574</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1868819</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>31-Oct-2024</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1905701</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
-        </is>
-      </c>
+          <t>21-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>Lahore's choking smog problem resonates in Punjab Assembly</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1868517</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>30-Oct-2024</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>The smog issue of Lahore resonated in the Punjab Assembly on Tuesday and Speaker Malik Muhammad Ahmed Khan decided to hold a special sitting on the matter on</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1870214</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Terror suspect held, another injured on Lahore's Barki Road - Dawn</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1897926</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>15-Mar-2025</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Lahore Ring Road closed ahead of PTI's protest - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1874184</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>23-Nov-2024</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Killing for a 'cause': Lahore shooter does it for Umrah tickets - Dawn</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1883631</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>07-Jan-2025</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>LAHORE: Sabzazar police have arrested a young man identified as Usman, accused of killing Muhammad Riaz on Jan 1 in exchange for two Umrah</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Lahore continues to grapple with smog - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1869904</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>05-Nov-2024</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>The Punjab government had closed all primary schools of Lahore due to the smog till Nov 9 and some private organisations started work from home</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1869475</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Govt moves to counter PTI protests as Lahore braces for showdown</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1863171</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>05-Oct-2024</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>A showdown between the PTI and the Punjab government in Lahore today (Saturday) appears almost certain as the party plans to hold a protest at Minar-i-Pakistan.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Shared crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1869042</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>01-Nov-2024</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1860210</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>21-Sept-2024</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1860210</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>21-Sept-2024</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Shared crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1869042</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>01-Nov-2024</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1905701</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
-        </is>
-      </c>
+          <t>21-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Schools set to reopen across Punjab, except Lahore, Multan - Dawn</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1873357</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>19-Nov-2024</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>The Punjab government on Monday announced reopening of schools across the province, except Lahore and Multan divisions, from Tuesday (today) in the wake of</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1260,1156 +1248,2490 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>31-Oct-2024</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Suspect held for allegedly raping college student in Lahore: police</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1864994</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>13-Oct-2024</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Lahore receives highest rainfall of last 30 years: Wasa - Dawn</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1845401</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>12-Jul-2024</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1865270</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1866011</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>18-Oct-2024</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>03-Jul-2025</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Lahore, AJK police recover 29 kidnapped children - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1865040</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>14-Oct-2024</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>LAHORE/MUZAFFARABAD: In a major breakthrough against child trafficking, a joint team of the Anti-Kidnap for Ransom Unit (AKRU) of the Lahore</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>3rd day of Punjab Assembly debate on smog: MPs for controlling ...</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1869234</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>02-Nov-2024</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>LAHORE: As the Punjab Assembly continued the debate on smog and water scarcity issues in the province for the third day here on Friday,</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>After Rawalpindi, Lahore makes helmets mandatory for pillion riders</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1889425</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>03-Feb-2025</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>LAHORE: Taking the lead from Rawalpindi, Lahore traffic police have also made helmets mandatory for pillion riders</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Lahore admin finalising spots for sacrificial animals' sale - Dawn</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1910442</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>12-May-2025</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>Lahore city district administration plans to make sacrificial animals sales points operational by May 20, as various arrangements are being finalised in this</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>A city in peril - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1874407</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>24-Nov-2024</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Reclaiming memory: Dera Tahli Sahib of Lahore - Newspaper - Dawn</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1896911</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>10-Mar-2025</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>LAHORE: The bloody Partition of 1947 resulted in the loss of tangible and intangible heritage for millions of</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Firm hands over Rs7.5m cheque to family of sacked worker who set ...</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1905674</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>21-Apr-2025</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>A multinational company (MNC) has paid a total amount of Rs7.5 million to the family of a former employee who died by suicide in Lahore earlier this year in</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1868870</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>31-Oct-2024</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>A city in peril - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1874407</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>24-Nov-2024</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Firm hands over Rs7.5m cheque to family of sacked worker who set ...</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1905674</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>21-Apr-2025</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>A multinational company (MNC) has paid a total amount of Rs7.5 million to the family of a former employee who died by suicide in Lahore earlier this year in</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>03-Jul-2025</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>UE VC removed for offending 'N' leader - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1857211</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>06-Sept-2024</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>LAHORE: The Punjab government on Thursday removed University of Education (UE) acting Vice Chancellor Prof Dr</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Punjab govt bids farewell to Lashari as WCLA chief on LHC's call</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1911055</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>15-May-2025</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>The Punjab government has accepted the resignation of Walled City of Lahore Authority (WCLA) Director-General Kamran Lashari after instructions from the Lahore</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Azerbaijan to set up trade centre in Lahore - Business - DAWN.COM</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1885071</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>14-Jan-2025</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>This was announced by Azerbaijan's Ambassador Khazar Farhadov during his speech at the Lahore Chamber of Commerce and Industry on Monday. “We</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Wildlife dept opposes plan to relocate exotic monkeys to Lahore</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1912261</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>21-May-2025</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Climate change ministry official claims Lahore zoo is suitable for monkeys seized by customs in January.</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Young Doctors Association to block main arteries in Lahore today</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1906459</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>25-Apr-2025</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>LAHORE: As the Pakistan Super League-X cricket matches started in Lahore on Thursday, the Young Doctors Association's (YDA) Punjab chapter</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>Critical care in crisis at Lahore's Mayo Hospital - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1850764</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>08-Aug-2024</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>LAHORE: Over a century-old Mayo Hospital is plagued by shortage of medicines, closure of several wards, suspension of diagnostic facilities</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Loadshedding worsens in Lahore as heatwave persists - Dawn</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1912083</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>20-May-2025</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>As the heatwave persists, various urban and rural areas of Lahore and adjoining districts have started experiencing hours-long loadshedding on a daily basis.</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Schemes to allot plots on security papers - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1875840</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>01-Dec-2024</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>LAHORE: On the direction of the National Accountability Bureau (NAB) Lahore, housing societies will now allot plots</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1865270</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1915235</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>04-Jun-2025</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Focal person posted for Lahore police, CCD coordination - Dawn</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1908480</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>05-May-2025</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>LAHORE: Capital City Police Officer Bilal Siddique Kamyana has appointed DIG administration Lahore Imran Kishwar as</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Medical college in Lahore oganises walk in support of army - Dawn</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1911175/medical-college-in-lahore-oganises-walk-in-support-of-army</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>15-May-2025</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>The Postgraduate Medical Institute (PGMI) organised a walk to express solidarity walk the Pakistan armed forces and</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>Can Lahore learn from London's Great Smog of 1952? - Dawn</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1873180</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>21-Nov-2024</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Lahore's deadly air could soon rival London's Great Smog — unless Pakistan follows the hard-earned lessons of the past.</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Leaders booked over pro-army rally in Lahore: PTI - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1911521</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>17-May-2025</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>LAHORE: The Pakistan Tehreek-i-Insaf (PTI) has claimed its leaders and workers have been booked for taking out a 'Pakistan Zindabad' rally,</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>19 die, 75 injured as windstorm, rain batter Punjab districts - Dawn</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1913140</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>25-May-2025</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>LAHORE: At least 19 people died while about 75 were injured as the heavy windstorm followed by rain battered various</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Fire at 220kV grid station in Lahore disrupts supply to several city ...</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1834687</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>21-May-2024</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>LAHORE: Almost half of the city plunged into darkness after the 220kV Sabzazar / Bund Road grid station caught fire causing a major</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Windstorm, rain disrupt Lahore's power supply - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1907845</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>02-May-2025</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>LAHORE: A strong windstorm followed by heavy to moderate rain brought relief from hot and humid conditions in the city on Thursday night.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Escaped lion attacks woman and children in Lahore - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1922087/escaped-lion-attacks-woman-and-children-in-lahore</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>04-Jul-2025</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Suspect held for allegedly raping college student in Lahore: police</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1864994</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>13-Oct-2024</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Art council, Ajoka theatre workshop from 16th - Newspaper - Dawn</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1924314/art-council-ajoka-theatre-workshop-from-16th</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>9 hours ago</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>LAHORE: The Alhamra Arts Council, in collaboration with Ajoka Theatre, is going to launch the second annual edition</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News ...</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1912424/pakistan-roundup-khuzdar-school-attack-india-blamed-pm-visits-quetta-dawn-news-english</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>21-May-2025</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>PkMAP protests Afghans' repatriation in Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1906860</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>27-Apr-2025</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Workers and supporters of the Pashtoonkhwa Milli Awami Party (PkMAP) took out a rally in support of Afghan refugees and urged the government of Pakistan to</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Two killed, 11 injured in explosion near Quetta: police - Dawn</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1914544</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>SHO identifies the deceased as Abdul Salam, owner of a coal mine, and his brother.</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>AKU concludes capacity building project with BAEC Quetta - Dawn</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1920867/aku-concludes-capacity-building-project-with-baec-quetta</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>29-Jun-2025</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>Project brought together professionals to build institutional capacity in designing and conducting large-scale, sample-based assessments.</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>1 dead, 10 injured in Quetta blast targeting convoy of PPP MPA Ali ...</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1911023</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>14-May-2025</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Lawmaker remains unhurt; Balochistan CM, govt spokesperson and Bilawal call for action against culprits, denounce attack.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>BNP-M demonstrators face tear gas, shelling amid sit-in near Quetta</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1902476</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>The Balochistan National Party-Mengal (BNP-M) on Sunday evening announced that police used tear gas and shelling to disperse protesters during their sit-in.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Three cops among six injured in grenade attack in Quetta - Dawn</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1915097</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>03-Jun-2025</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>Officials say unidentified assailants attacked a police vehicle with a hand-grenade near Bakra Mandi at the Eastern Bypass area of the</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Tear gas, water cannon employed to disperse Baloch Yakjehti ...</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1899479</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">03-Nov-2024 </t>
+          <t>22-Mar-2025</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from </t>
+          <t>Mahrang Baloch claims 3 killed, 13 others injured; Balochistan govt spokesperson says police took action to open road.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
+          <t>Quetta braces for BNP long march as impasse persists - Dawn</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1902347</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">31-Oct-2024 </t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on </t>
+          <t>BNP-M deadline for acceptance of its demands, including the release of Dr Mahrang Baloch, ended on Saturday midnight.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
+          <t>Quetta healthcare - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1890571</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Oct-2024 </t>
+          <t>08-Feb-2025</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>QUETTA, known for its changing weather patterns, often sees a surge in the number of patients requiring medical</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
+          <t>One killed, four injured in Quetta car blast - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865801</t>
+          <t>https://www.dawn.com/news/1914838</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">17-Oct-2024 </t>
+          <t>02-Jun-2025</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>Police say it was a targeted attack, in which a magnetic bomb was detonated remotely; responsibility not accepted by any group.</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Gun, bomb attacks claim three lives in Dera, Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1914636</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Apr-2025 </t>
+          <t>01-Jun-2025</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability </t>
+          <t>A Levies official was martyred in a shooting in Dera Bugti and a Levies police station was set on fire in Mastung district, while a roadside blast on the</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
+          <t>Quetta, 1935: Empire, earthquake, and the limits of control - Dawn</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1914296</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">15-Mar-2025 </t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>Research on the 1935 Quetta earthquake is shockingly limited, where anthropologists and historians can study colonial policies and</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>BNP-M reaches Kalat in march to Quetta against crackdown ... - Dawn</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1900877</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">18-Oct-2024 </t>
+          <t>28-Mar-2025</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on </t>
+          <t>The BNP-M had announced a long march from Wadh to Quetta today to protest against the arrests of Baloch Yakjehti Committee (BYC) leaders and activists.</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
+          <t>Indian boycott of Turkish goods condemned in Quetta - Dawn</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
+          <t>https://www.dawn.com/news/1911468</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">16-Oct-2024 </t>
+          <t>17-May-2025</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
+          <t>Traders say Pakistan aspires to have good trade relations with all countries.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Govt employees violently clash with police in Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1919872</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-Jun-2025 </t>
+          <t>25-Jun-2025</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion </t>
+          <t>QUETTA: Police arrested over two dozen government employees' on Tuesday after clashes erupted while they were protesting against their</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>26 martyred in Quetta railway station explosion - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1871371</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>10-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>At least 26 people, including 16 security personnel, lost their lives and 61 others were injured in a suicide bombing at a Quetta railway station on Saturday.</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>HBL PSL 2025: Abrar tears through Peshawar Zalmi batting ... - Dawn</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1903765</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>12-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>The mystery spinner gets 4 wickets as Peshawar get bundled out for 136 in their first outing; Quetta top-order fires to set up massive win.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Hindus in Quetta protest Indian accusations over Pahalgam attack</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1907649</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>01-May-2025</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Members of the Hindu community staged a protest rally in Quetta on Wednesday, condemning what they called baseless allegations against Pakistan by the Indian</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Four Frontier Corps personnel martyred, three injured in Quetta ...</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1906502</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>25-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Four Frontier Corps (FC) personnel were martyred and three other suffered injuries in an explosion near a security vehicle in Quetta's Margate area, police</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Unprivileged to get legal aid at state expense - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1924282</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Initiative to be implemented across all levels of the judiciary, from magistrate courts to the Supreme Court.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1900656</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>27-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Gas explosion claims two lives in Quetta - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1896528</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>08-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>A young girl and her mother were killed, while a minor boy was injured in an explosion inside a house near the Hazar Gangi area on the outskirts of the</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>President Zardari urges need to win 'war against terrorism' during ...</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1898968</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>19-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>President Asif Ali Zardari on Wednesday emphasised the need to win the “war against terrorism” at all costs during a visit to Quetta.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897237</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>11-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Protesters take away bodies from Quetta hospital morgue - Dawn</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1899300</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>21-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Authorities claim corpses belonged to Jaffar Express attackers; BYC activists say families had been protesting for days to see bodies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1914774</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>01-Jun-2025</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1900656</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>27-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897237</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>11-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Two Balochistan highways open for traffic after a week - Dawn</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1897163</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>11-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Traffic on Quetta-Karachi RCD Highway, Quetta-Taftan Highway (in Mastung), Karachi-Panjgur Highway, and Quetta-Sibi Highway had been blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Poet shot dead in Quetta - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1908757</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>06-May-2025</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Mir Allah Bakhsh Shahzad, a local Brahvi language poet and writer, was shot dead by unknown armed men in Sabzal Road area of the provincial capital on Monday.</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>ECP announces schedule for Quetta local bodies' polls - Dawn</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1915718</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>06-Jun-2025</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Returning officers will issue public notices on June 23; candidates can submit nomination papers between June 24 and 27.</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Footprints: GRIEF, ANGER RULE QUETTA STATION - Dawn</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1871777</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>12-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>A sombre mood prevails over the grandiose Quetta Railway Station. The whiff of carnage that took place here two days ago is palpable in the air.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>One hurt in grenade attack on Quetta police station - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1904124</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>14-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Police say unidentified motorcyclist hurled grenade at Kachi Baig police station, which exploded near the gate.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1901943</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>04-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1901943</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>04-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>'RDMC committed to empowering people through employment ...</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1924276/rdmc-committed-to-empowering-people-through-employment-education</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>QUETTA: Barrick Mining Corporation CEO Mark Bristow has reaffirmed Reko Diq Mining Company's (RDMC) commitment to empowering the people of</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>BNP supporters block Quetta-Karachi National Highway - Dawn</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1896255</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>07-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Hundreds of workers and supporters of the Balochistan National Party-Mengal blocked the Quetta-Karachi National Highway at Wadh, near Khuzdar, on Thursday in</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Quetta transport - Newspaper - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1840041</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>15-Jun-2024</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>SECTIONS of the press have reported that the federal government is not agreeable to allocating funds for the procurement of 100 buses for</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Balochistan govt warns BNP-M to limit march to Quetta's Sariab ...</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902266</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>05-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Balochistan government spokesperson Shahid Rind on Saturday offered the Balochistan National Party-Mengal (BNP-M) to march till Quetta's Shahwani Stadium on</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902827</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>08-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Quetta records 65 acts of terrorism in 2024 - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1881746</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>29-Dec-2024</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>QUETTA: As many as 365 people, including security personnel, have been martyred and several injured in terrorist attacks, targeted killings,</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Three killed, nine injured in road accidents - Newspaper - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1924281/three-killed-nine-injured-in-road-accidents</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>A pickup truck carrying a wedding party overturned near Chaman toll plaza, killing three people and injuring seven others, according to Levies</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902827</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>08-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1901075</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>29-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1806194</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>16-Jan-2024</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Armed men torch several govt buildings in Kalat - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1908061</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>03-May-2025</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Unknown armed men blocked the Quetta-Karachi Highway in the Mongochar area of Kalat district and set fire to several government buildings in the Mongochar</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Relatives not allowed to meet, deliver food to Mahrang Baloch in ...</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1899848</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>23-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Relatives are not being allowed to meet and deliver food to Dr Mahrang Baloch while she is in custody in Quetta District Jail, the Baloch Yakjehti Committee (</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902576</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>07-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Drinking water supply in Quetta restored - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1901936</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>04-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Official says water filtration plants in Duki, Pishin, Loralai and Kachhi to become fully operational by April 30.</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Night travel banned on key highways in Balochistan - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1901307</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>30-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>DC orders bar mostly public transport on arteries connecting Karachi, Sukkur, DI Khan, Multan to Quetta, Gwadar, and other cities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1903242</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>10-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1806194</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>16-Jan-2024</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>At Balochistan grand jirga, PM stresses need to win back 'misled ...</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1914525</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>31-May-2025</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Prime Minister Shehbaz Sharif on Saturday said that people who were “misled” by terrorists in Balochistan must be brought back on board.</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>HBL PSL 2025: Quetta Gladiators upstage Islamabad United ... - Dawn</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1908302</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>04-May-2025</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>LAHORE: Lady luck was smiling brightly on young Hasan Nawaz here at the Gaddafi Stadium Saturday night. It was a genuine thriller as in-form</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Journalists in Balochistan decry job cuts, censorship - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1908335</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>04-May-2025</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>The journalist community in Balochistan has called on the government to take urgent steps to ensure their safety, uphold press freedom, address widespread</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902576</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>07-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1903242</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>10-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865482</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>16-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1859465</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>17-Sept-2024</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Govt keeps BNP-M long march to Quetta at bay - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1902575</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>07-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Law enforcement personnel encircle sit-in to arrest Mengal; party calls for strike across Balochistan today.</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In ... - Dawn</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1900685</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>27-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In Quetta Market | Dawn News English.</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Journalists to observe black day today against Quetta incident - Dawn</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1834744</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>21-May-2024</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>KARACHI: Different factions of the Pakistan Federal Union of Journalists (PFUJ) and Karachi Union of Journalists</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>HBL PSL 2025: Quetta Gladiators upstage Islamabad United ... - Dawn</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1908302</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>04-May-2025</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>LAHORE: Lady luck was smiling brightly on young Hasan Nawaz here at the Gaddafi Stadium Saturday night. It was a genuine thriller as in-form</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Nine killed, over 50 injured in Quetta bus accident - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1862934</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>04-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Nine people were killed and over 50 others injured on Thursday when a bus carrying a wedding party veered off the road and fell into a ditch.</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Pipeline supplying gas to Quetta blown up - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1843307</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>02-Jul-2024</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>The miscreants used IED for blowing up the 12-inch pipeline,” a police officer told Dawn from Mach.</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865482</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>16-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Woman dies of Congo fever in Quetta - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1858850</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>14-Sept-2024</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>The patient was brought from Musakhail district in critical condition with suspected Congo virus and admitted to the Fatima Jinnah Chest</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Two killed, six injured as vehicle plunges into ravine along Quetta ...</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1857621</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>08-Sept-2024</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Officials say Inspector Jumma Khan of the Mineral Department was travelling to Zhob with his family when the vehicle veered off a narrow</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Balochistan ups security, anti-terror resolve - Newspaper - Dawn</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1871585</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>11-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Naqvi, Bugti briefed on initial investigation into station bombing; railway police register case.</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Centre rejects 100 green buses plan for Quetta - Pakistan - Dawn</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1838091</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>06-Jun-2024</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Balochistan is the only province that has no mass transit transport facility.</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Life comes to standstill across Balochistan amid strike - Dawn</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1874820</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>26-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Protesters seek child's recovery as schools, colleges stay shut; courts, roads remain deserted.</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1859465</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>17-Sept-2024</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Rally staged in Quetta for recovery of kidnapped tribesmen - Dawn</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1865038</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>14-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>QUETTA: Members of the Bugti Rabita Committee staged a demonstration on Sunday against the bandits of kacha area of Sindh, demanding</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Boy injured in Quetta blast - Pakistan - DAWN.COM</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>https://www.dawn.com/news/1905189</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>19-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>A 7-year-old boy was injured in a blast in the Hazar-Ganj area, located on the outskirts of Quetta, on Friday, police said.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
(fix): Fixing naming conventions
</commit_message>
<xml_diff>
--- a/DawnNews.xlsx
+++ b/DawnNews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,150 +480,154 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Over 3,800 vehicles of govt depts don't give a hoot to traffic laws in ...</t>
+          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1913330</t>
+          <t>https://www.dawn.com/news/1909625</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>26-May-2025</t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LAHORE: Over 3,800 official vehicles of the government departments being used by senior bureaucrats and police officers were found violating</t>
+          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>Over 3,800 vehicles of govt depts don't give a hoot to traffic laws in ...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1913330</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>18-Apr-2025</t>
+          <t>26-May-2025</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability</t>
+          <t>LAHORE: Over 3,800 official vehicles of the government departments being used by senior bureaucrats and police officers were found violating</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
+          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909625</t>
+          <t>https://www.dawn.com/news/1904992</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09-May-2025</t>
+          <t>18-Apr-2025</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
+          <t>Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Fast-food chain outlet attacked in Lahore's DHA - Pakistan - Dawn</t>
+          <t>Lahore police use water cannons to disperse young doctors - Dawn</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903292</t>
+          <t>https://www.dawn.com/news/1905123</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10-Apr-2025</t>
+          <t>19-Apr-2025</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LAHORE: An outlet of a fast-food chain on Wednesday came under an attack in Defense Housing Authority (DHA) when scores of people pelted it</t>
+          <t>LAHORE: The police used water cannons to disperse the protesting young doctors on the Mall Road, leaving two of the protesters,</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Public anger grows at traffic jams during PSL teams movement in ...</t>
+          <t>Fast-food chain outlet attacked in Lahore's DHA - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1907199</t>
+          <t>https://www.dawn.com/news/1903292</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>29-Apr-2025</t>
+          <t>10-Apr-2025</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LAHORE: Motorists and motorcyclists have run out of patience and started blaring horns during the movement of cricket teams participating in</t>
+          <t>LAHORE: An outlet of a fast-food chain on Wednesday came under an attack in Defense Housing Authority (DHA) when scores of people pelted it</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Latest - DAWN.COM</t>
+          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/latest-news</t>
+          <t>https://www.dawn.com/news/1892744</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Reaffirms commitment to Pak-China friendship; meets with foreign ministers of Iran, Uzbekistan, other SCO member states. Published about 8 hours ago</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>17-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lahore police use water cannons to disperse young doctors - Dawn</t>
+          <t>Public anger grows at traffic jams during PSL teams movement in ...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905123</t>
+          <t>https://www.dawn.com/news/1907199</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>19-Apr-2025</t>
+          <t>29-Apr-2025</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LAHORE: The police used water cannons to disperse the protesting young doctors on the Mall Road, leaving two of the protesters,</t>
+          <t>LAHORE: Motorists and motorcyclists have run out of patience and started blaring horns during the movement of cricket teams participating in</t>
         </is>
       </c>
     </row>
@@ -652,110 +656,106 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos</t>
+          <t>Latest - DAWN.COM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1892744</t>
+          <t>https://www.dawn.com/latest-news</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17-Mar-2025</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
-        </is>
-      </c>
+          <t>Meets PM Shehbaz in Islamabad, discusses exploring possible collaboration in defence production. Published about 11 hours ago</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
+          <t>People in Lahore celebrate Pakistan Army's victory over India - Dawn</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1887735</t>
+          <t>https://www.dawn.com/news/1910253</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>26-Jan-2025</t>
+          <t>11-May-2025</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
+          <t>LAHORE: People burst into celebrations after the armed forces early on Saturday responded to Indian war hysteria in a befitting manner and</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lahore High Court summons AGP in pleas against X ban - Dawn</t>
+          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902909</t>
+          <t>https://www.dawn.com/news/1887735</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>08-Apr-2025</t>
+          <t>26-Jan-2025</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>The Lahore High Court (LHC) on Tuesday summoned the Attorney General of Pakistan (AGP) Mansoor Usman Awan in a case pertaining to the ban on the social media</t>
+          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>People in Lahore celebrate Pakistan Army's victory over India - Dawn</t>
+          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1910253</t>
+          <t>https://www.dawn.com/news/1887735</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11-May-2025</t>
+          <t>26-Jan-2025</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LAHORE: People burst into celebrations after the armed forces early on Saturday responded to Indian war hysteria in a befitting manner and</t>
+          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English</t>
+          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909395</t>
+          <t>https://www.dawn.com/news/1870214</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>08-May-2025</t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
+          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
         </is>
       </c>
     </row>
@@ -784,34 +784,34 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lahore in the grip of a serious crisis - Newspaper - DAWN.COM</t>
+          <t>Lahore needs to do what London did - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870383</t>
+          <t>https://www.dawn.com/news/1873583</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>06-Nov-2024</t>
+          <t>20-Nov-2024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>On the Air Quality Index (AQI), Lahore has been consistently registering hazardous levels, surpassing major metropolitan cities, like New Delhi</t>
+          <t>THERE are severe threats to human health and environment that smog poses to Lahore and other cities in Punjab. Every</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
+          <t>Lahore in the grip of a serious crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870214</t>
+          <t>https://www.dawn.com/news/1870383</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -821,201 +821,201 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
+          <t>On the Air Quality Index (AQI), Lahore has been consistently registering hazardous levels, surpassing major metropolitan cities, like New Delhi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PTI moves LHC to seek permission for Lahore rally - Pakistan - Dawn</t>
+          <t>Lahore's air quality turns hazardous yet again - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1889622</t>
+          <t>https://www.dawn.com/news/1884188</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>04-Feb-2025</t>
+          <t>10-Jan-2025</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>The Pakistan Tehreek-i-Insaf on Monday approached the Lahore High Court, seeking permission to hold a public rally at the Minar-i-Pakistan on Feb 8.</t>
+          <t>LAHORE: The air quality in the provincial capital on Thursday again reached alarming levels, with its Air Quality Index (AQI) soaring to 529</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lahore needs to do what London did - Newspaper - DAWN.COM</t>
+          <t>Govt shuts primary schools in Lahore over record pollution - Dawn</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873583</t>
+          <t>https://www.dawn.com/news/1869574</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>20-Nov-2024</t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>THERE are severe threats to human health and environment that smog poses to Lahore and other cities in Punjab. Every</t>
+          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution - Dawn</t>
+          <t>PTI moves LHC to seek permission for Lahore rally - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1889622</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>03-Nov-2024</t>
+          <t>04-Feb-2025</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
+          <t>The Pakistan Tehreek-i-Insaf on Monday approached the Lahore High Court, seeking permission to hold a public rally at the Minar-i-Pakistan on Feb 8.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - Dawn</t>
+          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868819</t>
+          <t>https://www.dawn.com/news/1905701</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>31-Oct-2024</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
-        </is>
-      </c>
+          <t>21-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
+          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905701</t>
+          <t>https://www.dawn.com/news/1868819</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>31-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lahore's choking smog problem resonates in Punjab Assembly</t>
+          <t>Terror suspect held, another injured on Lahore's Barki Road - Dawn</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868517</t>
+          <t>https://www.dawn.com/news/1897926</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>30-Oct-2024</t>
+          <t>15-Mar-2025</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>The smog issue of Lahore resonated in the Punjab Assembly on Tuesday and Speaker Malik Muhammad Ahmed Khan decided to hold a special sitting on the matter on</t>
+          <t>LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
+          <t>Lahore's smog: the sun may be out but a sustainable solution ...</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870214</t>
+          <t>https://www.dawn.com/news/1875528</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>06-Nov-2024</t>
+          <t>29-Nov-2024</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
+          <t>In Lahore, the state-owned news agency, the Associated Press of Pakistan, reported 5,000 cases of asthma. “Frankly, this figure seems rather</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road - Dawn</t>
+          <t>Lahore Ring Road closed ahead of PTI's protest - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1874184</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15-Mar-2025</t>
+          <t>23-Nov-2024</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lahore Ring Road closed ahead of PTI's protest - Pakistan - Dawn</t>
+          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1874184</t>
+          <t>https://www.dawn.com/news/1870214</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>23-Nov-2024</t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>News and denials</t>
+          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
         </is>
       </c>
     </row>
@@ -1044,110 +1044,106 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lahore continues to grapple with smog - Pakistan - DAWN.COM</t>
+          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869904</t>
+          <t>https://www.dawn.com/news/1905701</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>05-Nov-2024</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>The Punjab government had closed all primary schools of Lahore due to the smog till Nov 9 and some private organisations started work from home</t>
-        </is>
-      </c>
+          <t>21-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+          <t>Govt moves to counter PTI protests as Lahore braces for showdown</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869475</t>
+          <t>https://www.dawn.com/news/1863171</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>03-Nov-2024</t>
+          <t>05-Oct-2024</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000</t>
+          <t>A showdown between the PTI and the Punjab government in Lahore today (Saturday) appears almost certain as the party plans to hold a protest at Minar-i-Pakistan.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Govt moves to counter PTI protests as Lahore braces for showdown</t>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1863171</t>
+          <t>https://www.dawn.com/news/1869475</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>05-Oct-2024</t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>A showdown between the PTI and the Punjab government in Lahore today (Saturday) appears almost certain as the party plans to hold a protest at Minar-i-Pakistan.</t>
+          <t>LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Shared crisis - Newspaper - DAWN.COM</t>
+          <t>Lahore continues to grapple with smog - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869042</t>
+          <t>https://www.dawn.com/news/1869904</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01-Nov-2024</t>
+          <t>05-Nov-2024</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
+          <t>The Punjab government had closed all primary schools of Lahore due to the smog till Nov 9 and some private organisations started work from home</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
+          <t>Shared crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1860210</t>
+          <t>https://www.dawn.com/news/1869042</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>21-Sept-2024</t>
+          <t>01-Nov-2024</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
+          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
         </is>
       </c>
     </row>
@@ -1176,106 +1172,110 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Shared crisis - Newspaper - DAWN.COM</t>
+          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869042</t>
+          <t>https://www.dawn.com/news/1868279</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01-Nov-2024</t>
+          <t>29-Oct-2024</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
+          <t>Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
+          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905701</t>
+          <t>https://www.dawn.com/news/1868870</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>31-Oct-2024</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Schools set to reopen across Punjab, except Lahore, Multan - Dawn</t>
+          <t>Shared crisis - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873357</t>
+          <t>https://www.dawn.com/news/1869042</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>19-Nov-2024</t>
+          <t>01-Nov-2024</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>The Punjab government on Monday announced reopening of schools across the province, except Lahore and Multan divisions, from Tuesday (today) in the wake of</t>
+          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
+          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1866011</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>31-Oct-2024</t>
+          <t>18-Oct-2024</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
+          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Suspect held for allegedly raping college student in Lahore: police</t>
+          <t>Schools set to reopen across Punjab, except Lahore, Multan - Dawn</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1864994</t>
+          <t>https://www.dawn.com/news/1873357</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>13-Oct-2024</t>
+          <t>19-Nov-2024</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
+          <t>The Punjab government on Monday announced reopening of schools across the province, except Lahore and Multan divisions, from Tuesday (today) in the wake of</t>
         </is>
       </c>
     </row>
@@ -1304,232 +1304,232 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
+          <t>Three Mayo Hospital nurses removed over injection deaths in Lahore</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1897329</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15-Oct-2024</t>
+          <t>12-Mar-2025</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>LAHORE: The Punjab health department has initiated proceedings under the Punjab Employees Efficiency, Discipline and Accountability (Peeda)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Lahore, AJK police recover 29 kidnapped children - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1865040</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>18-Oct-2024</t>
+          <t>14-Oct-2024</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
+          <t>LAHORE/MUZAFFARABAD: In a major breakthrough against child trafficking, a joint team of the Anti-Kidnap for Ransom Unit (AKRU) of the Lahore</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
+          <t>Lahore drug court directs urgent regulation of infant formula products</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
+          <t>https://www.dawn.com/news/1909619</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>03-Jul-2025</t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
+          <t>LAHORE: In a landmark judgment, the Drug Court Lahore has directed authorities to take urgent steps to regulate the manufacturing, sale, and</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Lahore, AJK police recover 29 kidnapped children - Pakistan - Dawn</t>
+          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865040</t>
+          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>14-Oct-2024</t>
+          <t>03-Jul-2025</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>LAHORE/MUZAFFARABAD: In a major breakthrough against child trafficking, a joint team of the Anti-Kidnap for Ransom Unit (AKRU) of the Lahore</t>
+          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3rd day of Punjab Assembly debate on smog: MPs for controlling ...</t>
+          <t>Murder on Lahore's Canal Road linked to underworld gang war</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869234</t>
+          <t>https://www.dawn.com/news/1856493</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>02-Nov-2024</t>
+          <t>03-Sept-2024</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LAHORE: As the Punjab Assembly continued the debate on smog and water scarcity issues in the province for the third day here on Friday,</t>
+          <t>LAHORE: The decades-old rivalry between two underworld dons of Lahore — Khwaja Gulshan alias Teefi Butt and the slain Arif Ameer alias Tipu</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>After Rawalpindi, Lahore makes helmets mandatory for pillion riders</t>
+          <t>3rd day of Punjab Assembly debate on smog: MPs for controlling ...</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1889425</t>
+          <t>https://www.dawn.com/news/1869234</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>03-Feb-2025</t>
+          <t>02-Nov-2024</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>LAHORE: Taking the lead from Rawalpindi, Lahore traffic police have also made helmets mandatory for pillion riders</t>
+          <t>LAHORE: As the Punjab Assembly continued the debate on smog and water scarcity issues in the province for the third day here on Friday,</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Lahore admin finalising spots for sacrificial animals' sale - Dawn</t>
+          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1910442</t>
+          <t>https://www.dawn.com/news/1865270</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>12-May-2025</t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Lahore city district administration plans to make sacrificial animals sales points operational by May 20, as various arrangements are being finalised in this</t>
+          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>A city in peril - Newspaper - DAWN.COM</t>
+          <t>After Rawalpindi, Lahore makes helmets mandatory for pillion riders</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1874407</t>
+          <t>https://www.dawn.com/news/1889425</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>24-Nov-2024</t>
+          <t>03-Feb-2025</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
+          <t>LAHORE: Taking the lead from Rawalpindi, Lahore traffic police have also made helmets mandatory for pillion riders</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Reclaiming memory: Dera Tahli Sahib of Lahore - Newspaper - Dawn</t>
+          <t>Lahore admin finalising spots for sacrificial animals' sale - Dawn</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1896911</t>
+          <t>https://www.dawn.com/news/1910442</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10-Mar-2025</t>
+          <t>12-May-2025</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>LAHORE: The bloody Partition of 1947 resulted in the loss of tangible and intangible heritage for millions of</t>
+          <t>Lahore city district administration plans to make sacrificial animals sales points operational by May 20, as various arrangements are being finalised in this</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Firm hands over Rs7.5m cheque to family of sacked worker who set ...</t>
+          <t>A city in peril - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905674</t>
+          <t>https://www.dawn.com/news/1874407</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
+          <t>24-Nov-2024</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>A multinational company (MNC) has paid a total amount of Rs7.5 million to the family of a former employee who died by suicide in Lahore earlier this year in</t>
+          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
+          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1868819</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1539,569 +1539,569 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
+          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>A city in peril - Newspaper - DAWN.COM</t>
+          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos ...</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1874407</t>
+          <t>https://www.dawn.com/news/1892744</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>24-Nov-2024</t>
+          <t>17-Mar-2025</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
+          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Firm hands over Rs7.5m cheque to family of sacked worker who set ...</t>
+          <t>Lahore receives highest rainfall of last 30 years: Wasa - Pakistan ...</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905674</t>
+          <t>https://www.dawn.com/news/1845401</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
+          <t>12-Jul-2024</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>A multinational company (MNC) has paid a total amount of Rs7.5 million to the family of a former employee who died by suicide in Lahore earlier this year in</t>
+          <t>While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
+          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
+          <t>https://www.dawn.com/news/1868279</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>03-Jul-2025</t>
+          <t>29-Oct-2024</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
+          <t>Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>UE VC removed for offending 'N' leader - Newspaper - DAWN.COM</t>
+          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English ...</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1857211</t>
+          <t>https://www.dawn.com/news/1909395</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>06-Sept-2024</t>
+          <t>08-May-2025</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>LAHORE: The Punjab government on Thursday removed University of Education (UE) acting Vice Chancellor Prof Dr</t>
+          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Punjab govt bids farewell to Lashari as WCLA chief on LHC's call</t>
+          <t>Suspect held for allegedly raping college student in Lahore: police ...</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911055</t>
+          <t>https://www.dawn.com/news/1864994</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15-May-2025</t>
+          <t>13-Oct-2024</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>The Punjab government has accepted the resignation of Walled City of Lahore Authority (WCLA) Director-General Kamran Lashari after instructions from the Lahore</t>
+          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Azerbaijan to set up trade centre in Lahore - Business - DAWN.COM</t>
+          <t>Lahore police probing claims about disinformation that sparked UK ...</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1885071</t>
+          <t>https://www.dawn.com/news/1853208</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14-Jan-2025</t>
+          <t>19-Aug-2024</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>This was announced by Azerbaijan's Ambassador Khazar Farhadov during his speech at the Lahore Chamber of Commerce and Industry on Monday. “We</t>
+          <t>Lahore Deputy Inspector General (Operations) Faisal Kamran told Dawn they were analysing the claims made by UK broadcaster ITV News and had</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Wildlife dept opposes plan to relocate exotic monkeys to Lahore</t>
+          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1912261</t>
+          <t>https://www.dawn.com/news/1869574</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>21-May-2025</t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Climate change ministry official claims Lahore zoo is suitable for monkeys seized by customs in January.</t>
+          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Young Doctors Association to block main arteries in Lahore today</t>
+          <t>Parking chaos deepens in Lahore as agencies pass the buck - Dawn</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1906459</t>
+          <t>https://www.dawn.com/news/1917362</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>25-Apr-2025</t>
+          <t>16-Jun-2025</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>LAHORE: As the Pakistan Super League-X cricket matches started in Lahore on Thursday, the Young Doctors Association's (YDA) Punjab chapter</t>
+          <t>The city's civic authorities appear to have no workable solution for Lahore's worsening parking crisis, with plans for setback areas in front of buildings and</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Critical care in crisis at Lahore's Mayo Hospital - Pakistan - Dawn</t>
+          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1850764</t>
+          <t>https://www.dawn.com/news/1909625</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>08-Aug-2024</t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>LAHORE: Over a century-old Mayo Hospital is plagued by shortage of medicines, closure of several wards, suspension of diagnostic facilities</t>
+          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Loadshedding worsens in Lahore as heatwave persists - Dawn</t>
+          <t>Leaders booked over pro-army rally in Lahore: PTI - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1912083</t>
+          <t>https://www.dawn.com/news/1911521</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>20-May-2025</t>
+          <t>17-May-2025</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>As the heatwave persists, various urban and rural areas of Lahore and adjoining districts have started experiencing hours-long loadshedding on a daily basis.</t>
+          <t>LAHORE: The Pakistan Tehreek-i-Insaf (PTI) has claimed its leaders and workers have been booked for taking out a 'Pakistan Zindabad' rally,</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Schemes to allot plots on security papers - Newspaper - DAWN.COM</t>
+          <t>19 die, 75 injured as windstorm, rain batter Punjab districts - Dawn</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1875840</t>
+          <t>https://www.dawn.com/news/1913140</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01-Dec-2024</t>
+          <t>25-May-2025</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>LAHORE: On the direction of the National Accountability Bureau (NAB) Lahore, housing societies will now allot plots</t>
+          <t>LAHORE: At least 19 people died while about 75 were injured as the heavy windstorm followed by rain battered various</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
+          <t>Fire at 220kV grid station in Lahore disrupts supply to several city ...</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1834687</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15-Oct-2024</t>
+          <t>21-May-2024</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>LAHORE: Almost half of the city plunged into darkness after the 220kV Sabzazar / Bund Road grid station caught fire causing a major</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
+          <t>Escaped lion attacks woman and children in Lahore - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915235</t>
+          <t>https://www.dawn.com/news/1922087/escaped-lion-attacks-woman-and-children-in-lahore</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>04-Jun-2025</t>
+          <t>04-Jul-2025</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Focal person posted for Lahore police, CCD coordination - Dawn</t>
+          <t>Art council, Ajoka theatre workshop from 16th - Newspaper - Dawn</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908480</t>
+          <t>https://www.dawn.com/news/1924314/art-council-ajoka-theatre-workshop-from-16th</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>05-May-2025</t>
+          <t>10 hours ago</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>LAHORE: Capital City Police Officer Bilal Siddique Kamyana has appointed DIG administration Lahore Imran Kishwar as</t>
+          <t>LAHORE: The Alhamra Arts Council, in collaboration with Ajoka Theatre, is going to launch the second annual edition</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Medical college in Lahore oganises walk in support of army - Dawn</t>
+          <t>Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News ...</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911175/medical-college-in-lahore-oganises-walk-in-support-of-army</t>
+          <t>https://www.dawn.com/news/1912424/pakistan-roundup-khuzdar-school-attack-india-blamed-pm-visits-quetta-dawn-news-english</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15-May-2025</t>
+          <t>21-May-2025</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>The Postgraduate Medical Institute (PGMI) organised a walk to express solidarity walk the Pakistan armed forces and</t>
+          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Can Lahore learn from London's Great Smog of 1952? - Dawn</t>
+          <t>PkMAP protests Afghans' repatriation in Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873180</t>
+          <t>https://www.dawn.com/news/1906860</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>21-Nov-2024</t>
+          <t>27-Apr-2025</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Lahore's deadly air could soon rival London's Great Smog — unless Pakistan follows the hard-earned lessons of the past.</t>
+          <t>Workers and supporters of the Pashtoonkhwa Milli Awami Party (PkMAP) took out a rally in support of Afghan refugees and urged the government of Pakistan to</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Leaders booked over pro-army rally in Lahore: PTI - Pakistan - Dawn</t>
+          <t>BNP-M demonstrators face tear gas, shelling amid sit-in near Quetta</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911521</t>
+          <t>https://www.dawn.com/news/1902476</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17-May-2025</t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>LAHORE: The Pakistan Tehreek-i-Insaf (PTI) has claimed its leaders and workers have been booked for taking out a 'Pakistan Zindabad' rally,</t>
+          <t>The Balochistan National Party-Mengal (BNP-M) on Sunday evening announced that police used tear gas and shelling to disperse protesters during their sit-in.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>19 die, 75 injured as windstorm, rain batter Punjab districts - Dawn</t>
+          <t>Two killed, 11 injured in explosion near Quetta: police - Dawn</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1913140</t>
+          <t>https://www.dawn.com/news/1914544</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>25-May-2025</t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>LAHORE: At least 19 people died while about 75 were injured as the heavy windstorm followed by rain battered various</t>
+          <t>SHO identifies the deceased as Abdul Salam, owner of a coal mine, and his brother.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Fire at 220kV grid station in Lahore disrupts supply to several city ...</t>
+          <t>AKU concludes capacity building project with BAEC Quetta - Dawn</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1834687</t>
+          <t>https://www.dawn.com/news/1920867/aku-concludes-capacity-building-project-with-baec-quetta</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>29-Jun-2025</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>LAHORE: Almost half of the city plunged into darkness after the 220kV Sabzazar / Bund Road grid station caught fire causing a major</t>
+          <t>Project brought together professionals to build institutional capacity in designing and conducting large-scale, sample-based assessments.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Windstorm, rain disrupt Lahore's power supply - Pakistan - Dawn</t>
+          <t>Three cops among six injured in grenade attack in Quetta - Dawn</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1907845</t>
+          <t>https://www.dawn.com/news/1915097</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>02-May-2025</t>
+          <t>03-Jun-2025</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>LAHORE: A strong windstorm followed by heavy to moderate rain brought relief from hot and humid conditions in the city on Thursday night.</t>
+          <t>Officials say unidentified assailants attacked a police vehicle with a hand-grenade near Bakra Mandi at the Eastern Bypass area of the</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Escaped lion attacks woman and children in Lahore - Pakistan - Dawn</t>
+          <t>1 dead, 10 injured in Quetta blast targeting convoy of PPP MPA Ali ...</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1922087/escaped-lion-attacks-woman-and-children-in-lahore</t>
+          <t>https://www.dawn.com/news/1911023</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>04-Jul-2025</t>
+          <t>14-May-2025</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>News and denials</t>
+          <t>Lawmaker remains unhurt; Balochistan CM, govt spokesperson and Bilawal call for action against culprits, denounce attack.</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Suspect held for allegedly raping college student in Lahore: police</t>
+          <t>Tear gas, water cannon employed to disperse Baloch Yakjehti ...</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1864994</t>
+          <t>https://www.dawn.com/news/1899479</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>13-Oct-2024</t>
+          <t>22-Mar-2025</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
+          <t>Mahrang Baloch claims 3 killed, 13 others injured; Balochistan govt spokesperson says police took action to open road.</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Art council, Ajoka theatre workshop from 16th - Newspaper - Dawn</t>
+          <t>Quetta braces for BNP long march as impasse persists - Dawn</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924314/art-council-ajoka-theatre-workshop-from-16th</t>
+          <t>https://www.dawn.com/news/1902347</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>9 hours ago</t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>LAHORE: The Alhamra Arts Council, in collaboration with Ajoka Theatre, is going to launch the second annual edition</t>
+          <t>BNP-M deadline for acceptance of its demands, including the release of Dr Mahrang Baloch, ended on Saturday midnight.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News ...</t>
+          <t>Quetta healthcare - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1912424/pakistan-roundup-khuzdar-school-attack-india-blamed-pm-visits-quetta-dawn-news-english</t>
+          <t>https://www.dawn.com/news/1890571</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>21-May-2025</t>
+          <t>08-Feb-2025</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News English.</t>
+          <t>QUETTA, known for its changing weather patterns, often sees a surge in the number of patients requiring medical</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>PkMAP protests Afghans' repatriation in Quetta - Pakistan - Dawn</t>
+          <t>One killed, four injured in Quetta car blast - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1906860</t>
+          <t>https://www.dawn.com/news/1914838</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27-Apr-2025</t>
+          <t>02-Jun-2025</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Workers and supporters of the Pashtoonkhwa Milli Awami Party (PkMAP) took out a rally in support of Afghan refugees and urged the government of Pakistan to</t>
+          <t>Police say it was a targeted attack, in which a magnetic bomb was detonated remotely; responsibility not accepted by any group.</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Two killed, 11 injured in explosion near Quetta: police - Dawn</t>
+          <t>Quetta, 1935: Empire, earthquake, and the limits of control - Dawn</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914544</t>
+          <t>https://www.dawn.com/news/1914296</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2111,719 +2111,719 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>SHO identifies the deceased as Abdul Salam, owner of a coal mine, and his brother.</t>
+          <t>Research on the 1935 Quetta earthquake is shockingly limited, where anthropologists and historians can study colonial policies and</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>AKU concludes capacity building project with BAEC Quetta - Dawn</t>
+          <t>Gun, bomb attacks claim three lives in Dera, Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1920867/aku-concludes-capacity-building-project-with-baec-quetta</t>
+          <t>https://www.dawn.com/news/1914636</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>29-Jun-2025</t>
+          <t>01-Jun-2025</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Project brought together professionals to build institutional capacity in designing and conducting large-scale, sample-based assessments.</t>
+          <t>A Levies official was martyred in a shooting in Dera Bugti and a Levies police station was set on fire in Mastung district, while a roadside blast on the</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>1 dead, 10 injured in Quetta blast targeting convoy of PPP MPA Ali ...</t>
+          <t>BNP-M reaches Kalat in march to Quetta against crackdown ... - Dawn</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911023</t>
+          <t>https://www.dawn.com/news/1900877</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14-May-2025</t>
+          <t>28-Mar-2025</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Lawmaker remains unhurt; Balochistan CM, govt spokesperson and Bilawal call for action against culprits, denounce attack.</t>
+          <t>The BNP-M had announced a long march from Wadh to Quetta today to protest against the arrests of Baloch Yakjehti Committee (BYC) leaders and activists.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>BNP-M demonstrators face tear gas, shelling amid sit-in near Quetta</t>
+          <t>Indian boycott of Turkish goods condemned in Quetta - Dawn</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902476</t>
+          <t>https://www.dawn.com/news/1911468</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>06-Apr-2025</t>
+          <t>17-May-2025</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>The Balochistan National Party-Mengal (BNP-M) on Sunday evening announced that police used tear gas and shelling to disperse protesters during their sit-in.</t>
+          <t>Traders say Pakistan aspires to have good trade relations with all countries.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Three cops among six injured in grenade attack in Quetta - Dawn</t>
+          <t>Govt employees violently clash with police in Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915097</t>
+          <t>https://www.dawn.com/news/1919872</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>03-Jun-2025</t>
+          <t>25-Jun-2025</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Officials say unidentified assailants attacked a police vehicle with a hand-grenade near Bakra Mandi at the Eastern Bypass area of the</t>
+          <t>QUETTA: Police arrested over two dozen government employees' on Tuesday after clashes erupted while they were protesting against their</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Tear gas, water cannon employed to disperse Baloch Yakjehti ...</t>
+          <t>HBL PSL 2025: Abrar tears through Peshawar Zalmi batting ... - Dawn</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899479</t>
+          <t>https://www.dawn.com/news/1903765</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>22-Mar-2025</t>
+          <t>12-Apr-2025</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Mahrang Baloch claims 3 killed, 13 others injured; Balochistan govt spokesperson says police took action to open road.</t>
+          <t>The mystery spinner gets 4 wickets as Peshawar get bundled out for 136 in their first outing; Quetta top-order fires to set up massive win.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Quetta braces for BNP long march as impasse persists - Dawn</t>
+          <t>26 martyred in Quetta railway station explosion - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902347</t>
+          <t>https://www.dawn.com/news/1871371</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>06-Apr-2025</t>
+          <t>10-Nov-2024</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>BNP-M deadline for acceptance of its demands, including the release of Dr Mahrang Baloch, ended on Saturday midnight.</t>
+          <t>At least 26 people, including 16 security personnel, lost their lives and 61 others were injured in a suicide bombing at a Quetta railway station on Saturday.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Quetta healthcare - Newspaper - DAWN.COM</t>
+          <t>Hindus in Quetta protest Indian accusations over Pahalgam attack</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1890571</t>
+          <t>https://www.dawn.com/news/1907649</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>08-Feb-2025</t>
+          <t>01-May-2025</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>QUETTA, known for its changing weather patterns, often sees a surge in the number of patients requiring medical</t>
+          <t>Members of the Hindu community staged a protest rally in Quetta on Wednesday, condemning what they called baseless allegations against Pakistan by the Indian</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>One killed, four injured in Quetta car blast - Pakistan - DAWN.COM</t>
+          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914838</t>
+          <t>https://www.dawn.com/news/1900656</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>02-Jun-2025</t>
+          <t>27-Mar-2025</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Police say it was a targeted attack, in which a magnetic bomb was detonated remotely; responsibility not accepted by any group.</t>
+          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Gun, bomb attacks claim three lives in Dera, Quetta - Pakistan - Dawn</t>
+          <t>Unprivileged to get legal aid at state expense - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914636</t>
+          <t>https://www.dawn.com/news/1924282</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>01-Jun-2025</t>
+          <t>10 hours ago</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>A Levies official was martyred in a shooting in Dera Bugti and a Levies police station was set on fire in Mastung district, while a roadside blast on the</t>
+          <t>Initiative to be implemented across all levels of the judiciary, from magistrate courts to the Supreme Court.</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Quetta, 1935: Empire, earthquake, and the limits of control - Dawn</t>
+          <t>Gas explosion claims two lives in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914296</t>
+          <t>https://www.dawn.com/news/1896528</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>31-May-2025</t>
+          <t>08-Mar-2025</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Research on the 1935 Quetta earthquake is shockingly limited, where anthropologists and historians can study colonial policies and</t>
+          <t>A young girl and her mother were killed, while a minor boy was injured in an explosion inside a house near the Hazar Gangi area on the outskirts of the</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>BNP-M reaches Kalat in march to Quetta against crackdown ... - Dawn</t>
+          <t>Four Frontier Corps personnel martyred, three injured in Quetta ...</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900877</t>
+          <t>https://www.dawn.com/news/1906502</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>28-Mar-2025</t>
+          <t>25-Apr-2025</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>The BNP-M had announced a long march from Wadh to Quetta today to protest against the arrests of Baloch Yakjehti Committee (BYC) leaders and activists.</t>
+          <t>Four Frontier Corps (FC) personnel were martyred and three other suffered injuries in an explosion near a security vehicle in Quetta's Margate area, police</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Indian boycott of Turkish goods condemned in Quetta - Dawn</t>
+          <t>President Zardari urges need to win 'war against terrorism' during ...</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911468</t>
+          <t>https://www.dawn.com/news/1898968</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>17-May-2025</t>
+          <t>19-Mar-2025</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Traders say Pakistan aspires to have good trade relations with all countries.</t>
+          <t>President Asif Ali Zardari on Wednesday emphasised the need to win the “war against terrorism” at all costs during a visit to Quetta.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Govt employees violently clash with police in Quetta - Pakistan - Dawn</t>
+          <t>Protesters take away bodies from Quetta hospital morgue - Dawn</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1919872</t>
+          <t>https://www.dawn.com/news/1899300</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>25-Jun-2025</t>
+          <t>21-Mar-2025</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>QUETTA: Police arrested over two dozen government employees' on Tuesday after clashes erupted while they were protesting against their</t>
+          <t>Authorities claim corpses belonged to Jaffar Express attackers; BYC activists say families had been protesting for days to see bodies.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>26 martyred in Quetta railway station explosion - Pakistan - Dawn</t>
+          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1871371</t>
+          <t>https://www.dawn.com/news/1914774</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10-Nov-2024</t>
+          <t>01-Jun-2025</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>At least 26 people, including 16 security personnel, lost their lives and 61 others were injured in a suicide bombing at a Quetta railway station on Saturday.</t>
+          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>HBL PSL 2025: Abrar tears through Peshawar Zalmi batting ... - Dawn</t>
+          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903765</t>
+          <t>https://www.dawn.com/news/1897237</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>12-Apr-2025</t>
+          <t>11-Mar-2025</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>The mystery spinner gets 4 wickets as Peshawar get bundled out for 136 in their first outing; Quetta top-order fires to set up massive win.</t>
+          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Hindus in Quetta protest Indian accusations over Pahalgam attack</t>
+          <t>PIA to resume direct flights from Quetta to Jeddah - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1907649</t>
+          <t>https://www.dawn.com/news/1846448</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>01-May-2025</t>
+          <t>18-Jul-2024</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Members of the Hindu community staged a protest rally in Quetta on Wednesday, condemning what they called baseless allegations against Pakistan by the Indian</t>
+          <t>Pakistan International Airlines (PIA) on Thursday announced that it will resume direct flights from Quetta to the Saudi Arabian capital of Jeddah from next</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Four Frontier Corps personnel martyred, three injured in Quetta ...</t>
+          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1906502</t>
+          <t>https://www.dawn.com/news/1914774</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>25-Apr-2025</t>
+          <t>01-Jun-2025</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Four Frontier Corps (FC) personnel were martyred and three other suffered injuries in an explosion near a security vehicle in Quetta's Margate area, police</t>
+          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Unprivileged to get legal aid at state expense - Pakistan - DAWN.COM</t>
+          <t>Footprints: GRIEF, ANGER RULE QUETTA STATION - Dawn</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924282</t>
+          <t>https://www.dawn.com/news/1871777</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>12-Nov-2024</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Initiative to be implemented across all levels of the judiciary, from magistrate courts to the Supreme Court.</t>
+          <t>A sombre mood prevails over the grandiose Quetta Railway Station. The whiff of carnage that took place here two days ago is palpable in the air.</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
+          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900656</t>
+          <t>https://www.dawn.com/news/1901943</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>27-Mar-2025</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
-        </is>
-      </c>
+          <t>04-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Gas explosion claims two lives in Quetta - Pakistan - DAWN.COM</t>
+          <t>BNP supporters block Quetta-Karachi National Highway - Dawn</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1896528</t>
+          <t>https://www.dawn.com/news/1896255</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>08-Mar-2025</t>
+          <t>07-Mar-2025</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>A young girl and her mother were killed, while a minor boy was injured in an explosion inside a house near the Hazar Gangi area on the outskirts of the</t>
+          <t>Hundreds of workers and supporters of the Balochistan National Party-Mengal blocked the Quetta-Karachi National Highway at Wadh, near Khuzdar, on Thursday in</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>President Zardari urges need to win 'war against terrorism' during ...</t>
+          <t>One hurt in grenade attack on Quetta police station - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1898968</t>
+          <t>https://www.dawn.com/news/1904124</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>19-Mar-2025</t>
+          <t>14-Apr-2025</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>President Asif Ali Zardari on Wednesday emphasised the need to win the “war against terrorism” at all costs during a visit to Quetta.</t>
+          <t>Police say unidentified motorcyclist hurled grenade at Kachi Baig police station, which exploded near the gate.</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
+          <t>Balochistan govt warns BNP-M to limit march to Quetta's Sariab ...</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897237</t>
+          <t>https://www.dawn.com/news/1902266</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>11-Mar-2025</t>
+          <t>05-Apr-2025</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
+          <t>Balochistan government spokesperson Shahid Rind on Saturday offered the Balochistan National Party-Mengal (BNP-M) to march till Quetta's Shahwani Stadium on</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Protesters take away bodies from Quetta hospital morgue - Dawn</t>
+          <t>Two Balochistan highways open for traffic after a week - Dawn</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899300</t>
+          <t>https://www.dawn.com/news/1897163</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>21-Mar-2025</t>
+          <t>11-Mar-2025</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Authorities claim corpses belonged to Jaffar Express attackers; BYC activists say families had been protesting for days to see bodies.</t>
+          <t>Traffic on Quetta-Karachi RCD Highway, Quetta-Taftan Highway (in Mastung), Karachi-Panjgur Highway, and Quetta-Sibi Highway had been blocked</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
+          <t>Quetta-Sibi road reopened after gun battle in Bolan - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914774</t>
+          <t>https://www.dawn.com/news/1893896</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>01-Jun-2025</t>
+          <t>24-Feb-2025</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
+          <t>Three militants were killed in an hour-long exchange of fire between security forces and two armed groups which had blocked the Quetta-Sibi highway.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
+          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900656</t>
+          <t>https://www.dawn.com/news/1902827</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>27-Mar-2025</t>
+          <t>08-Apr-2025</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
+          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
+          <t>Poet shot dead in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897237</t>
+          <t>https://www.dawn.com/news/1908757</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11-Mar-2025</t>
+          <t>06-May-2025</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
+          <t>Mir Allah Bakhsh Shahzad, a local Brahvi language poet and writer, was shot dead by unknown armed men in Sabzal Road area of the provincial capital on Monday.</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Two Balochistan highways open for traffic after a week - Dawn</t>
+          <t>ECP announces schedule for Quetta local bodies' polls - Dawn</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897163</t>
+          <t>https://www.dawn.com/news/1915718</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11-Mar-2025</t>
+          <t>06-Jun-2025</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Traffic on Quetta-Karachi RCD Highway, Quetta-Taftan Highway (in Mastung), Karachi-Panjgur Highway, and Quetta-Sibi Highway had been blocked</t>
+          <t>Returning officers will issue public notices on June 23; candidates can submit nomination papers between June 24 and 27.</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Poet shot dead in Quetta - Pakistan - DAWN.COM</t>
+          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908757</t>
+          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>06-May-2025</t>
+          <t>10 hours ago</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Mir Allah Bakhsh Shahzad, a local Brahvi language poet and writer, was shot dead by unknown armed men in Sabzal Road area of the provincial capital on Monday.</t>
+          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>ECP announces schedule for Quetta local bodies' polls - Dawn</t>
+          <t>Quetta transport - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915718</t>
+          <t>https://www.dawn.com/news/1840041</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>06-Jun-2025</t>
+          <t>15-Jun-2024</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Returning officers will issue public notices on June 23; candidates can submit nomination papers between June 24 and 27.</t>
+          <t>SECTIONS of the press have reported that the federal government is not agreeable to allocating funds for the procurement of 100 buses for</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Footprints: GRIEF, ANGER RULE QUETTA STATION - Dawn</t>
+          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1871777</t>
+          <t>https://www.dawn.com/news/1901075</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>12-Nov-2024</t>
+          <t>29-Mar-2025</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>A sombre mood prevails over the grandiose Quetta Railway Station. The whiff of carnage that took place here two days ago is palpable in the air.</t>
+          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>One hurt in grenade attack on Quetta police station - Pakistan - Dawn</t>
+          <t>Quetta records 65 acts of terrorism in 2024 - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904124</t>
+          <t>https://www.dawn.com/news/1881746</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>14-Apr-2025</t>
+          <t>29-Dec-2024</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Police say unidentified motorcyclist hurled grenade at Kachi Baig police station, which exploded near the gate.</t>
+          <t>QUETTA: As many as 365 people, including security personnel, have been martyred and several injured in terrorist attacks, targeted killings,</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
+          <t>'RDMC committed to empowering people through employment ...</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901943</t>
+          <t>https://www.dawn.com/news/1924276</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>04-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr"/>
+          <t>10 hours ago</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>QUETTA: Barrick Mining Corporation CEO Mark Bristow has reaffirmed Reko Diq Mining Company's (RDMC) commitment to empowering the people of</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
+          <t>Three killed, nine injured in road accidents - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
+          <t>https://www.dawn.com/news/1924281/three-killed-nine-injured-in-road-accidents</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2833,443 +2833,447 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
+          <t>A pickup truck carrying a wedding party overturned near Chaman toll plaza, killing three people and injuring seven others, according to Levies</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
+          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901943</t>
+          <t>https://www.dawn.com/news/1901075</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>04-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr"/>
+          <t>29-Mar-2025</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
+          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
+          <t>https://www.dawn.com/news/1806194</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>16-Jan-2024</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
+          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>'RDMC committed to empowering people through employment ...</t>
+          <t>Armed men torch several govt buildings in Kalat - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924276/rdmc-committed-to-empowering-people-through-employment-education</t>
+          <t>https://www.dawn.com/news/1908061</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>03-May-2025</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>QUETTA: Barrick Mining Corporation CEO Mark Bristow has reaffirmed Reko Diq Mining Company's (RDMC) commitment to empowering the people of</t>
+          <t>Unknown armed men blocked the Quetta-Karachi Highway in the Mongochar area of Kalat district and set fire to several government buildings in the Mongochar</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>BNP supporters block Quetta-Karachi National Highway - Dawn</t>
+          <t>Relatives not allowed to meet, deliver food to Mahrang Baloch in ...</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1896255</t>
+          <t>https://www.dawn.com/news/1899848</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>07-Mar-2025</t>
+          <t>23-Mar-2025</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Hundreds of workers and supporters of the Balochistan National Party-Mengal blocked the Quetta-Karachi National Highway at Wadh, near Khuzdar, on Thursday in</t>
+          <t>Relatives are not being allowed to meet and deliver food to Dr Mahrang Baloch while she is in custody in Quetta District Jail, the Baloch Yakjehti Committee (</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Quetta transport - Newspaper - DAWN.COM</t>
+          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1840041</t>
+          <t>https://www.dawn.com/news/1902576</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15-Jun-2024</t>
+          <t>07-Apr-2025</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>SECTIONS of the press have reported that the federal government is not agreeable to allocating funds for the procurement of 100 buses for</t>
+          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Balochistan govt warns BNP-M to limit march to Quetta's Sariab ...</t>
+          <t>Woman dies of Congo fever in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902266</t>
+          <t>https://www.dawn.com/news/1858850</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>05-Apr-2025</t>
+          <t>14-Sept-2024</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Balochistan government spokesperson Shahid Rind on Saturday offered the Balochistan National Party-Mengal (BNP-M) to march till Quetta's Shahwani Stadium on</t>
+          <t>The patient was brought from Musakhail district in critical condition with suspected Congo virus and admitted to the Fatima Jinnah Chest</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
+          <t>Snowfall in Balochistan disrupts traffic - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902827</t>
+          <t>https://www.dawn.com/news/1886462</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>08-Apr-2025</t>
+          <t>20-Jan-2025</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
+          <t>Heavy rain and snowfall disrupted transportation across several towns and cities in Balochistan, while residents of Quetta faced severe hardships.</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Quetta records 65 acts of terrorism in 2024 - Pakistan - DAWN.COM</t>
+          <t>Drinking water supply in Quetta restored - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1881746</t>
+          <t>https://www.dawn.com/news/1901936</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>29-Dec-2024</t>
+          <t>04-Apr-2025</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>QUETTA: As many as 365 people, including security personnel, have been martyred and several injured in terrorist attacks, targeted killings,</t>
+          <t>Official says water filtration plants in Duki, Pishin, Loralai and Kachhi to become fully operational by April 30.</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Three killed, nine injured in road accidents - Newspaper - DAWN.COM</t>
+          <t>New polio case found in Quetta, taking this year's tally to 33 - Dawn</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924281/three-killed-nine-injured-in-road-accidents</t>
+          <t>https://www.dawn.com/news/1865282</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>A pickup truck carrying a wedding party overturned near Chaman toll plaza, killing three people and injuring seven others, according to Levies</t>
+          <t>According to an official of the Regional Reference Laboratory for Polio Eradication at the National Institute of Health Islamabad, the wild</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
+          <t>Field Marshal Asim Munir assails India's 'hydro-terrorism ... - Dawn</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902827</t>
+          <t>https://www.dawn.com/news/1914324</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>08-Apr-2025</t>
+          <t>30-May-2025</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
+          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir on Friday emphasised the need for a peaceful resolution to the Kashmir dispute, assailing India's “unlawful</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
+          <t>Two killed, six injured as vehicle plunges into ravine along Quetta ...</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901075</t>
+          <t>https://www.dawn.com/news/1857621</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>29-Mar-2025</t>
+          <t>08-Sept-2024</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
+          <t>Officials say Inspector Jumma Khan of the Mineral Department was travelling to Zhob with his family when the vehicle veered off a narrow</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
+          <t>Journalists in Balochistan decry job cuts, censorship - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1806194</t>
+          <t>https://www.dawn.com/news/1908335</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16-Jan-2024</t>
+          <t>04-May-2025</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
+          <t>The journalist community in Balochistan has called on the government to take urgent steps to ensure their safety, uphold press freedom, address widespread</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Armed men torch several govt buildings in Kalat - Pakistan - Dawn</t>
+          <t>Plan finalised to increase Quetta Metropolitan Corporation's revenue</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908061</t>
+          <t>https://www.dawn.com/news/1875870</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>03-May-2025</t>
+          <t>01-Dec-2024</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Unknown armed men blocked the Quetta-Karachi Highway in the Mongochar area of Kalat district and set fire to several government buildings in the Mongochar</t>
+          <t>QUETTA: Quetta Metropolitan Corporation (QMC) Administrator Muhammad Hamza Shafqaat has said a a strategy has been finalised to increase QMC</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Relatives not allowed to meet, deliver food to Mahrang Baloch in ...</t>
+          <t>Night travel banned on key highways in Balochistan - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899848</t>
+          <t>https://www.dawn.com/news/1901307</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>23-Mar-2025</t>
+          <t>30-Mar-2025</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Relatives are not being allowed to meet and deliver food to Dr Mahrang Baloch while she is in custody in Quetta District Jail, the Baloch Yakjehti Committee (</t>
+          <t>DC orders bar mostly public transport on arteries connecting Karachi, Sukkur, DI Khan, Multan to Quetta, Gwadar, and other cities.</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
+          <t>At Balochistan grand jirga, PM stresses need to win back 'misled ...</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902576</t>
+          <t>https://www.dawn.com/news/1914525</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>07-Apr-2025</t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
+          <t>Prime Minister Shehbaz Sharif on Saturday said that people who were “misled” by terrorists in Balochistan must be brought back on board.</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Drinking water supply in Quetta restored - Pakistan - DAWN.COM</t>
+          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901936</t>
+          <t>https://www.dawn.com/news/1903242</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>04-Apr-2025</t>
+          <t>10-Apr-2025</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Official says water filtration plants in Duki, Pishin, Loralai and Kachhi to become fully operational by April 30.</t>
+          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Night travel banned on key highways in Balochistan - Pakistan - Dawn</t>
+          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901307</t>
+          <t>https://www.dawn.com/news/1865482</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>30-Mar-2025</t>
+          <t>16-Oct-2024</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>DC orders bar mostly public transport on arteries connecting Karachi, Sukkur, DI Khan, Multan to Quetta, Gwadar, and other cities.</t>
+          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
+          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In ... - Dawn</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903242</t>
+          <t>https://www.dawn.com/news/1900685</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>10-Apr-2025</t>
+          <t>27-Mar-2025</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
+          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In Quetta Market | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
+          <t>Govt keeps BNP-M long march to Quetta at bay - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1806194</t>
+          <t>https://www.dawn.com/news/1902575</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16-Jan-2024</t>
+          <t>07-Apr-2025</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
+          <t>Law enforcement personnel encircle sit-in to arrest Mengal; party calls for strike across Balochistan today.</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>At Balochistan grand jirga, PM stresses need to win back 'misled ...</t>
+          <t>Journalists to observe black day today against Quetta incident - Dawn</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914525</t>
+          <t>https://www.dawn.com/news/1834744</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>31-May-2025</t>
+          <t>21-May-2024</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Prime Minister Shehbaz Sharif on Saturday said that people who were “misled” by terrorists in Balochistan must be brought back on board.</t>
+          <t>KARACHI: Different factions of the Pakistan Federal Union of Journalists (PFUJ) and Karachi Union of Journalists</t>
         </is>
       </c>
     </row>
@@ -3298,440 +3302,220 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Journalists in Balochistan decry job cuts, censorship - Pakistan - Dawn</t>
+          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908335</t>
+          <t>https://www.dawn.com/news/1859465</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>04-May-2025</t>
+          <t>17-Sept-2024</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>The journalist community in Balochistan has called on the government to take urgent steps to ensure their safety, uphold press freedom, address widespread</t>
+          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
+          <t>Cop martyred, 6 injured in blast near ATF vehicle in Quetta: police</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902576</t>
+          <t>https://www.dawn.com/news/1898108</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>07-Apr-2025</t>
+          <t>15-Mar-2025</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
+          <t>Vehicle belongs to Anti-Terrorist Force; three of the personnel seriously injured, says medical superintendent at Bolan Medical Complex.</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
+          <t>Rally staged in Quetta for recovery of kidnapped tribesmen - Dawn</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903242</t>
+          <t>https://www.dawn.com/news/1865038</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10-Apr-2025</t>
+          <t>14-Oct-2024</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
+          <t>QUETTA: Members of the Bugti Rabita Committee staged a demonstration on Sunday against the bandits of kacha area of Sindh, demanding</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
+          <t>Missing persons' camp burnt down in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865482</t>
+          <t>https://www.dawn.com/news/1870633</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>16-Oct-2024</t>
+          <t>07-Nov-2024</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
+          <t>Unidentified individuals set fire to the main camp of the Voice for Baloch Missing Persons (VBMP) near Quetta Press Club on Wednesday.</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
+          <t>Methane explosion traps 12 inside coal mine near Quetta - Dawn</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1859465</t>
+          <t>https://www.dawn.com/news/1884221</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>17-Sept-2024</t>
+          <t>10-Jan-2025</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
+          <t>QUETTA: At least 12 coal miners were trapped inside a mine after an explosion caused by methane gas in the Sanjdi coal field area, around 40</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Govt keeps BNP-M long march to Quetta at bay - Pakistan - Dawn</t>
+          <t>4 bodies recovered, search continues for 8 others after mine ... - Dawn</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902575</t>
+          <t>https://www.dawn.com/news/1884307</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>07-Apr-2025</t>
+          <t>10-Jan-2025</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Law enforcement personnel encircle sit-in to arrest Mengal; party calls for strike across Balochistan today.</t>
+          <t>The bodies of four miners were recovered on Friday during a rescue operation near a coal mine in Quetta after a dozen mineworkers were left trapped therein.</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In ... - Dawn</t>
+          <t>Complete shutdown in Quetta over student's kidnapping - Dawn</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900685</t>
+          <t>https://www.dawn.com/news/1873571</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27-Mar-2025</t>
+          <t>20-Nov-2024</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In Quetta Market | Dawn News English.</t>
+          <t>A complete shutdown was observed in the provincial capital on Tuesday in protest against the kidnapping of an 11-year-old student.</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Journalists to observe black day today against Quetta incident - Dawn</t>
+          <t>Centre rejects 100 green buses plan for Quetta - Pakistan - Dawn</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1834744</t>
+          <t>https://www.dawn.com/news/1838091</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>06-Jun-2024</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>KARACHI: Different factions of the Pakistan Federal Union of Journalists (PFUJ) and Karachi Union of Journalists</t>
+          <t>Balochistan is the only province that has no mass transit transport facility.</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>HBL PSL 2025: Quetta Gladiators upstage Islamabad United ... - Dawn</t>
+          <t>The killer highways of Balochistan - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908302</t>
+          <t>https://www.dawn.com/news/1895508</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>04-May-2025</t>
+          <t>05-Mar-2025</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>LAHORE: Lady luck was smiling brightly on young Hasan Nawaz here at the Gaddafi Stadium Saturday night. It was a genuine thriller as in-form</t>
+          <t>“Is the road safe?” Muhammad Ahmed, who was travelling from Quetta to Dera Ismail Khan after 15 long years, asked the bus driver. News over</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Nine killed, over 50 injured in Quetta bus accident - Pakistan - Dawn</t>
+          <t>Protests persist in Balochistan against alleged rigging - Dawn</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1862934</t>
+          <t>https://www.dawn.com/news/1814552</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>04-Oct-2024</t>
+          <t>16-Feb-2024</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Nine people were killed and over 50 others injured on Thursday when a bus carrying a wedding party veered off the road and fell into a ditch.</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>Pipeline supplying gas to Quetta blown up - Pakistan - DAWN.COM</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1843307</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>The miscreants used IED for blowing up the 12-inch pipeline,” a police officer told Dawn from Mach.</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1865482</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>16-Oct-2024</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Woman dies of Congo fever in Quetta - Pakistan - DAWN.COM</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1858850</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>14-Sept-2024</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>The patient was brought from Musakhail district in critical condition with suspected Congo virus and admitted to the Fatima Jinnah Chest</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Two killed, six injured as vehicle plunges into ravine along Quetta ...</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1857621</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>08-Sept-2024</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>Officials say Inspector Jumma Khan of the Mineral Department was travelling to Zhob with his family when the vehicle veered off a narrow</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Balochistan ups security, anti-terror resolve - Newspaper - Dawn</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1871585</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>11-Nov-2024</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>Naqvi, Bugti briefed on initial investigation into station bombing; railway police register case.</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>Centre rejects 100 green buses plan for Quetta - Pakistan - Dawn</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1838091</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>06-Jun-2024</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>Balochistan is the only province that has no mass transit transport facility.</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Life comes to standstill across Balochistan amid strike - Dawn</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1874820</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>26-Nov-2024</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Protesters seek child's recovery as schools, colleges stay shut; courts, roads remain deserted.</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1859465</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>17-Sept-2024</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>Rally staged in Quetta for recovery of kidnapped tribesmen - Dawn</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1865038</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>14-Oct-2024</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>QUETTA: Members of the Bugti Rabita Committee staged a demonstration on Sunday against the bandits of kacha area of Sindh, demanding</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Boy injured in Quetta blast - Pakistan - DAWN.COM</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1905189</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>19-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>A 7-year-old boy was injured in a blast in the Hazar-Ganj area, located on the outskirts of Quetta, on Friday, police said.</t>
+          <t>QUETTA: Supporters of</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
(fix): Fixing CAPTCHA solver.
</commit_message>
<xml_diff>
--- a/DawnNews.xlsx
+++ b/DawnNews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,2073 +458,2069 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Parking chaos deepens in Lahore as agencies pass the buck - Dawn</t>
+          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1917362</t>
+          <t>https://www.dawn.com/news/1869475</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>16-Jun-2025</t>
+          <t>03-Nov-2024</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The city's civic authorities appear to have no workable solution for Lahore's worsening parking crisis, with plans for setback areas in front of buildings and</t>
+          <t>LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
+          <t>Punjab govt declares smog as 'calamity', sends children with ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909625</t>
+          <t>https://www.dawn.com/news/1868870</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09-May-2025</t>
+          <t>31-Oct-2024</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
+          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Over 3,800 vehicles of govt depts don't give a hoot to traffic laws in ...</t>
+          <t>Over 250 arrested as protests against alleged Lahore rape spread to ...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1913330</t>
+          <t>https://www.dawn.com/news/1865801</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>26-May-2025</t>
+          <t>17-Oct-2024</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LAHORE: Over 3,800 official vehicles of the government departments being used by senior bureaucrats and police officers were found violating</t>
+          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
+          <t>28 hurt as police come down hard on student protest in Lahore ...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904992</t>
+          <t>https://www.dawn.com/news/1865270</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>18-Apr-2025</t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability</t>
+          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lahore police use water cannons to disperse young doctors - Dawn</t>
+          <t>Terror suspect held, another injured on Lahore's Barki Road ...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905123</t>
+          <t>https://www.dawn.com/news/1897926</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>19-Apr-2025</t>
+          <t>15-Mar-2025</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LAHORE: The police used water cannons to disperse the protesting young doctors on the Mall Road, leaving two of the protesters,</t>
+          <t>LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Fast-food chain outlet attacked in Lahore's DHA - Pakistan - Dawn</t>
+          <t>Lahore High Court Bar for barring Ahmadis from practising Islamic ...</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903292</t>
+          <t>https://www.dawn.com/news/1915235</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10-Apr-2025</t>
+          <t>04-Jun-2025</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LAHORE: An outlet of a fast-food chain on Wednesday came under an attack in Defense Housing Authority (DHA) when scores of people pelted it</t>
+          <t>The Lahore High Court Bar Association (LHCBA) has asked the Punjab police chief to prevent Ahmadiyya community from observing Islamic rituals on the occasion</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos</t>
+          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1892744</t>
+          <t>https://www.dawn.com/news/1866011</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>17-Mar-2025</t>
+          <t>18-Oct-2024</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
+          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Public anger grows at traffic jams during PSL teams movement in ...</t>
+          <t>Murder on Lahore's Canal Road linked to underworld gang war ...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1907199</t>
+          <t>https://www.dawn.com/news/1856493</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>29-Apr-2025</t>
+          <t>03-Sept-2024</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LAHORE: Motorists and motorcyclists have run out of patience and started blaring horns during the movement of cricket teams participating in</t>
+          <t>LAHORE: The decades-old rivalry between two underworld dons of Lahore — Khwaja Gulshan alias Teefi Butt and the slain Arif Ameer alias Tipu</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Two more bodies of Libya boat tragedy victims arrive in Lahore - Dawn</t>
+          <t>Lahore, AJK police recover 29 kidnapped children - Pakistan ...</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908386</t>
+          <t>https://www.dawn.com/news/1865040</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>04-May-2025</t>
+          <t>14-Oct-2024</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Two more bodies of Pakistan nationals who lost their lives in a tragic boat accident off the eastern coast of Libya, arrived at Lahore Airport on Sunday.</t>
+          <t>LAHORE/MUZAFFARABAD: In a major breakthrough against child trafficking, a joint team of the Anti-Kidnap for Ransom Unit (AKRU) of the Lahore</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Latest - DAWN.COM</t>
+          <t>University student allegedly gang-raped in Lahore - Pakistan ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/latest-news</t>
+          <t>https://www.dawn.com/news/1886857</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Meets PM Shehbaz in Islamabad, discusses exploring possible collaboration in defence production. Published about 11 hours ago</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>22-Jan-2025</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>A female student of a leading private university of Lahore was allegedly gang-raped by three suspects in a flat in a private housing society located on Raiwind</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>People in Lahore celebrate Pakistan Army's victory over India - Dawn</t>
+          <t>Lahore students stage anti-harassment rally against alleged campus ...</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1910253</t>
+          <t>https://www.dawn.com/news/1865392</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11-May-2025</t>
+          <t>15-Oct-2024</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>LAHORE: People burst into celebrations after the armed forces early on Saturday responded to Indian war hysteria in a befitting manner and</t>
+          <t>On Sunday, a security guard was arrested after news related to the incident went viral on social media. According to a police statement, the</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
+          <t>'Justice must prevail': Celebrities outraged after alleged rape of ...</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1887735</t>
+          <t>https://images.dawn.com/news/1192852/justice-must-prevail-celebrities-outraged-after-alleged-rape-of-lahore-college-student</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>26-Jan-2025</t>
+          <t>16-Oct-2024</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
+          <t>Celebrities are speaking out after a security guard allegedly raped a student at a private college in Lahore. They're calling for justice.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Unkind reality of Lahore winters - Newspaper - DAWN.COM</t>
+          <t>Lahore may face more polluted air in days ahead - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1887735</t>
+          <t>https://www.dawn.com/news/1870214</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>26-Jan-2025</t>
+          <t>06-Nov-2024</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>The winter this year in Lahore has been a little more intense than usual, adding to the woes of the city's homeless, who have been facing a heartbreaking</t>
+          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
+          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870214</t>
+          <t>https://www.dawn.com/news/1860210</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>06-Nov-2024</t>
+          <t>21-Sept-2024</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
+          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lahore High Court summons AGP in pleas against X ban - Dawn</t>
+          <t>Escaped lion attacks woman and children in Lahore - Pakistan ...</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902909</t>
+          <t>https://www.dawn.com/news/1922087/escaped-lion-attacks-woman-and-children-in-lahore</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>08-Apr-2025</t>
+          <t>04-Jul-2025</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>The Lahore High Court (LHC) on Tuesday summoned the Attorney General of Pakistan (AGP) Mansoor Usman Awan in a case pertaining to the ban on the social media</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lahore needs to do what London did - Newspaper - DAWN.COM</t>
+          <t>Lahore-based coworking startup Colabs raises $2m in pre Series A ...</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873583</t>
+          <t>https://www.dawn.com/news/1867329</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>20-Nov-2024</t>
+          <t>24-Oct-2024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>THERE are severe threats to human health and environment that smog poses to Lahore and other cities in Punjab. Every</t>
+          <t>The startup announced that it had “raised an additional $2m in pre-series A, bringing the total to over $5m in venture capital funding from top investors”.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lahore in the grip of a serious crisis - Newspaper - DAWN.COM</t>
+          <t>Lahore's smog: the sun may be out but a sustainable solution ...</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870383</t>
+          <t>https://www.dawn.com/news/1875528</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>06-Nov-2024</t>
+          <t>29-Nov-2024</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>On the Air Quality Index (AQI), Lahore has been consistently registering hazardous levels, surpassing major metropolitan cities, like New Delhi</t>
+          <t>In Lahore, the state-owned news agency, the Associated Press of Pakistan, reported 5,000 cases of asthma. “Frankly, this figure seems rather</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lahore's air quality turns hazardous yet again - Pakistan - DAWN.COM</t>
+          <t>Killing for a 'cause': Lahore shooter does it for Umrah tickets ...</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1884188</t>
+          <t>https://www.dawn.com/news/1883631</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10-Jan-2025</t>
+          <t>07-Jan-2025</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>LAHORE: The air quality in the provincial capital on Thursday again reached alarming levels, with its Air Quality Index (AQI) soaring to 529</t>
+          <t>LAHORE: Sabzazar police have arrested a young man identified as Usman, accused of killing Muhammad Riaz on Jan 1 in exchange for two Umrah</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution - Dawn</t>
+          <t>Lahore submerged as rain breaks 44-year record - Newspaper ...</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1849532</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>03-Nov-2024</t>
+          <t>02-Aug-2024</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
+          <t>A rare spell of torrential monsoon rain inundated Lahore, breaking a 44-year record in just three hours, six people across the country lost their lives in rain</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PTI moves LHC to seek permission for Lahore rally - Pakistan - Dawn</t>
+          <t>Can Lahore learn from London's Great Smog of 1952? - Pakistan ...</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1889622</t>
+          <t>https://www.dawn.com/news/1873180</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>04-Feb-2025</t>
+          <t>21-Nov-2024</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>The Pakistan Tehreek-i-Insaf on Monday approached the Lahore High Court, seeking permission to hold a public rally at the Minar-i-Pakistan on Feb 8.</t>
+          <t>Lahore's deadly air could soon rival London's Great Smog — unless Pakistan follows the hard-earned lessons of the past.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
+          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905701</t>
+          <t>https://www.dawn.com/news/1860210</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>21-Sept-2024</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - Dawn</t>
+          <t>CM Maryam catches flak for 'humiliating' Lahore's Mayo Hospital ...</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868819</t>
+          <t>https://www.dawn.com/news/1896514</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>31-Oct-2024</t>
+          <t>08-Mar-2025</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
+          <t>LAHORE: A video clip showing Chief Minister Maryam Nawaz snubbing the medical superintendent of the Mayo Hospital went viral on Friday,</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Terror suspect held, another injured on Lahore's Barki Road - Dawn</t>
+          <t>Lahore's air quality shows slight improvement as it drops out of ...</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897926</t>
+          <t>https://www.dawn.com/news/1872991</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15-Mar-2025</t>
+          <t>17-Nov-2024</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>LAHORE: The security forces arrested a 'possible' suicide bomber and injured another after crossfire on Barki Road on Friday night.</t>
+          <t>Lahore's Air Quality Index (AQI) ranking on Sunday showed a slight improvement as it dropped out of the “hazardous” category for the first time in 12 days.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lahore's smog: the sun may be out but a sustainable solution ...</t>
+          <t>Lahore's challenge - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1875528</t>
+          <t>https://www.dawn.com/news/1850167</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>29-Nov-2024</t>
+          <t>05-Aug-2024</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>In Lahore, the state-owned news agency, the Associated Press of Pakistan, reported 5,000 cases of asthma. “Frankly, this figure seems rather</t>
+          <t>Presently, Lahore is 60 per cent concretised, putting it in a precarious spot, with dangerously high temperatures and an anaemic drainage system</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lahore Ring Road closed ahead of PTI's protest - Pakistan - Dawn</t>
+          <t>Lahore's air quality turns hazardous yet again - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1874184</t>
+          <t>https://www.dawn.com/news/1884188</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>23-Nov-2024</t>
+          <t>10-Jan-2025</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>News and denials</t>
+          <t>LAHORE: The air quality in the provincial capital on Thursday again reached alarming levels, with its Air Quality Index (AQI) soaring to 529</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lahore may face more polluted air in days ahead - Pakistan - Dawn</t>
+          <t>People in Lahore celebrate Pakistan Army's victory over India ...</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870214</t>
+          <t>https://www.dawn.com/news/1910253</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>06-Nov-2024</t>
+          <t>11-May-2025</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Environmental experts predicted that the AQI could further spike between 600 and 700 from Nov 6 to 8, as polluted winds from India are expected to contribute</t>
+          <t>LAHORE: People burst into celebrations after the armed forces early on Saturday responded to Indian war hysteria in a befitting manner and</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Killing for a 'cause': Lahore shooter does it for Umrah tickets - Dawn</t>
+          <t>Probe finds over 200 kanal land was illegally transferred to Bahria ...</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1883631</t>
+          <t>https://www.dawn.com/news/1904992</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>07-Jan-2025</t>
+          <t>18-Apr-2025</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>LAHORE: Sabzazar police have arrested a young man identified as Usman, accused of killing Muhammad Riaz on Jan 1 in exchange for two Umrah</t>
+          <t>Over 200 kanal land of a cooperative housing society was illegally transferred to property tycoon Malik Riaz's Bahria Town Lahore, the National Accountability</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Overseas Pakistani woman attacked in Lahore's factory area: police</t>
+          <t>High AQI levels persist in Lahore despite smog-specific steps ...</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1905701</t>
+          <t>https://www.dawn.com/news/1870858</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>21-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
+          <t>08-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LAHORE: The provincial metropolis's air pollution on Thursday reached unprecedented levels, ranking it as the world's most polluted city for</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Govt moves to counter PTI protests as Lahore braces for showdown</t>
+          <t>Lahore continues to grapple with smog - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1863171</t>
+          <t>https://www.dawn.com/news/1869904</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>05-Oct-2024</t>
+          <t>05-Nov-2024</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>A showdown between the PTI and the Punjab government in Lahore today (Saturday) appears almost certain as the party plans to hold a protest at Minar-i-Pakistan.</t>
+          <t>The Punjab government had closed all primary schools of Lahore due to the smog till Nov 9 and some private organisations started work from home</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lahore's AQI touches unprecedented level - Pakistan - DAWN.COM</t>
+          <t>Lahore High Court summons replies from DC, others on Aurat March ...</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869475</t>
+          <t>https://www.dawn.com/news/1888444/lahore-high-court-summons-replies-from-dc-others-on-aurat-march-contempt-petition</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>03-Nov-2024</t>
+          <t>29-Jan-2025</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LAHORE: Air pollution in Lahore soared on Saturday, with the Air Quality Index (AQI) briefly reaching an “unprecedented” level of over 1,000</t>
+          <t>Latest Celebrity Culture Comment Local Her. DAWN · Latest · Celebrity · Culture ArtBooksFilm &amp; TVMusicNewsParentingRightsReviewsStyle</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Lahore continues to grapple with smog - Pakistan - DAWN.COM</t>
+          <t>Public anger grows at traffic jams during PSL teams movement in ...</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869904</t>
+          <t>https://www.dawn.com/news/1907199</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>05-Nov-2024</t>
+          <t>29-Apr-2025</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>The Punjab government had closed all primary schools of Lahore due to the smog till Nov 9 and some private organisations started work from home</t>
+          <t>LAHORE: Motorists and motorcyclists have run out of patience and started blaring horns during the movement of cricket teams participating in</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Shared crisis - Newspaper - DAWN.COM</t>
+          <t>Lahore Ring Road closed ahead of PTI's protest - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869042</t>
+          <t>https://www.dawn.com/news/1874184</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01-Nov-2024</t>
+          <t>23-Nov-2024</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Anti-climactic end to PTI's Lahore power show as police clear stage ...</t>
+          <t>High-speed trains to reduce Pindi, Lahore travel time to two hours ...</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1860210</t>
+          <t>https://www.dawn.com/news/1915044</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>21-Sept-2024</t>
+          <t>03-Jun-2025</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>KP CM Gandapur did not reach rally as people began to clear venue after deadline; government ministers take digs at power show's end.</t>
+          <t>RAWALPINDI: Minister for Railways Hanif Abbasi on Monday said the speed of trains between Rawalpindi and Lahore will</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - Dawn</t>
+          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan ...</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868279</t>
+          <t>https://www.dawn.com/news/1909625</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>29-Oct-2024</t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its</t>
+          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Punjab govt declares smog as 'calamity', sends children with ... - Dawn</t>
+          <t>Probe finds Lahore rape story fabricated, spread via fake accounts ...</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868870</t>
+          <t>https://www.dawn.com/news/1866108</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>31-Oct-2024</t>
+          <t>19-Oct-2024</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>The Environmental Protection Agency (EPA) ordered all special education schools in Lahore to send students with conditions/diseases susceptible to poor air on</t>
+          <t>The committee report available with Dawn revealed that the news of the rape was fabricated and spread via fake social media accounts to create unrest and a law</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Shared crisis - Newspaper - DAWN.COM</t>
+          <t>30 students injured as Punjab University guards pounce on their ...</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869042</t>
+          <t>https://www.dawn.com/news/1867001</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01-Nov-2024</t>
+          <t>23-Oct-2024</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>WITH Lahore experiencing unprecedented levels of smog, the Punjab government has announced a series of “green</t>
+          <t>LAHORE: Thirty students were injured in the torture by security guards of the Punjab University as they attacked the participants in</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>No student has any evidence of alleged Lahore rape, Punjab AG ...</t>
+          <t>Govt moves to counter PTI protests as Lahore braces for showdown ...</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1866011</t>
+          <t>https://www.dawn.com/news/1863171</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>18-Oct-2024</t>
+          <t>05-Oct-2024</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Punjab Chief Minister Maryam Nawaz has declared that the alleged rape was “fabricated news”, blaming the PTI for spreading the “fake reports” on</t>
+          <t>A showdown between the PTI and the Punjab government in Lahore today (Saturday) appears almost certain as the party plans to hold a protest at Minar-i-Pakistan.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Schools set to reopen across Punjab, except Lahore, Multan - Dawn</t>
+          <t>PTI moves LHC to seek permission for Lahore rally - Pakistan ...</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873357</t>
+          <t>https://www.dawn.com/news/1889622</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>19-Nov-2024</t>
+          <t>04-Feb-2025</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>The Punjab government on Monday announced reopening of schools across the province, except Lahore and Multan divisions, from Tuesday (today) in the wake of</t>
+          <t>The Pakistan Tehreek-i-Insaf on Monday approached the Lahore High Court, seeking permission to hold a public rally at the Minar-i-Pakistan on Feb 8.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Lahore receives highest rainfall of last 30 years: Wasa - Dawn</t>
+          <t>Lahore court discharges suspect in UK riots disinformation case ...</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1845401</t>
+          <t>https://www.dawn.com/news/1854866</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>12-Jul-2024</t>
+          <t>26-Aug-2024</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding</t>
+          <t>UK broadcaster ITV News had asserted that a Pakistani individual was the originator of the false news story. Farhan Asif was taken into custody</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Three Mayo Hospital nurses removed over injection deaths in Lahore</t>
+          <t>Punjab to spend Rs250bn in three years on Pindi-Lahore fast train ...</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897329</t>
+          <t>https://www.dawn.com/news/1919949</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>12-Mar-2025</t>
+          <t>25-Jun-2025</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>LAHORE: The Punjab health department has initiated proceedings under the Punjab Employees Efficiency, Discipline and Accountability (Peeda)</t>
+          <t>Due to the special attention of Prime Minister Shahbaz Sharif, great good news will soon come out in Pakistan Railways sector. Without the</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Lahore, AJK police recover 29 kidnapped children - Pakistan - Dawn</t>
+          <t>Marquee owner booked for serving 'toxic' food in Lahore - Pakistan ...</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865040</t>
+          <t>https://www.dawn.com/news/1891554</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14-Oct-2024</t>
+          <t>13-Feb-2025</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>LAHORE/MUZAFFARABAD: In a major breakthrough against child trafficking, a joint team of the Anti-Kidnap for Ransom Unit (AKRU) of the Lahore</t>
+          <t>LAHORE: The Punjab Food Authority got a first information report lodged against the owner of a marquee at Johar Town when its management</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Lahore drug court directs urgent regulation of infant formula products</t>
+          <t>Plane makes emergency landing at Lahore airport - Newspaper ...</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909619</t>
+          <t>https://www.dawn.com/news/1860731</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>09-May-2025</t>
+          <t>24-Sept-2024</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>LAHORE: In a landmark judgment, the Drug Court Lahore has directed authorities to take urgent steps to regulate the manufacturing, sale, and</t>
+          <t>LAHORE: A private airline's plane had to make an emergency landing at the Allama Iqbal International Airport here</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TikToker held with 13 guards for 'public display of arms' in Lahore</t>
+          <t>Lahore's choking smog problem resonates in Punjab Assembly ...</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1921826/tiktoker-held-with-13-guards-for-public-display-of-arms-in-lahore</t>
+          <t>https://www.dawn.com/news/1868517</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>03-Jul-2025</t>
+          <t>30-Oct-2024</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>LAHORE: The Crime Control Department (CCD) of Lahore police on Wednesday arrested a known TikToker and his 13 security guards for “public</t>
+          <t>The smog issue of Lahore resonated in the Punjab Assembly on Tuesday and Speaker Malik Muhammad Ahmed Khan decided to hold a special sitting on the matter on</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Murder on Lahore's Canal Road linked to underworld gang war</t>
+          <t>Heavy Fog Enveloped Lahore | Breaking News | Dawn News ...</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1856493</t>
+          <t>https://www.dawn.com/news/1882624</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>03-Sept-2024</t>
+          <t>02-Jan-2025</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LAHORE: The decades-old rivalry between two underworld dons of Lahore — Khwaja Gulshan alias Teefi Butt and the slain Arif Ameer alias Tipu</t>
+          <t>Heavy Fog Enveloped Lahore | Breaking News | Dawn News.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3rd day of Punjab Assembly debate on smog: MPs for controlling ...</t>
+          <t>'Tech-savvy' robbers block cell signals, loot Rs15m from house in ...</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869234</t>
+          <t>https://www.dawn.com/news/1867201</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>02-Nov-2024</t>
+          <t>24-Oct-2024</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>LAHORE: As the Punjab Assembly continued the debate on smog and water scarcity issues in the province for the third day here on Friday,</t>
+          <t>LAHORE: A five-member gang of robbers looted valuables, including gold ornaments and cash worth over Rs15 million from a house in Defence as</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>28 hurt as police come down hard on student protest in Lahore - Dawn</t>
+          <t>Young Doctors Association to block main arteries in Lahore today ...</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865270</t>
+          <t>https://www.dawn.com/news/1906459</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15-Oct-2024</t>
+          <t>25-Apr-2025</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Conflicting accounts emerge as officials, college admin deny alleged rape; CM forms probe body.</t>
+          <t>LAHORE: As the Pakistan Super League-X cricket matches started in Lahore on Thursday, the Young Doctors Association's (YDA) Punjab chapter</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>After Rawalpindi, Lahore makes helmets mandatory for pillion riders</t>
+          <t>'Tech-savvy' robbers block cell signals, loot Rs15m from house in ...</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1889425</t>
+          <t>https://www.dawn.com/news/1867201</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>03-Feb-2025</t>
+          <t>24-Oct-2024</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>LAHORE: Taking the lead from Rawalpindi, Lahore traffic police have also made helmets mandatory for pillion riders</t>
+          <t>LAHORE: A five-member gang of robbers looted valuables, including gold ornaments and cash worth over Rs15 million from a house in Defence as</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Lahore admin finalising spots for sacrificial animals' sale - Dawn</t>
+          <t>Over 3,800 vehicles of govt depts don't give a hoot to traffic laws in ...</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1910442</t>
+          <t>https://www.dawn.com/news/1913330</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>12-May-2025</t>
+          <t>26-May-2025</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Lahore city district administration plans to make sacrificial animals sales points operational by May 20, as various arrangements are being finalised in this</t>
+          <t>LAHORE: Over 3,800 official vehicles of the government departments being used by senior bureaucrats and police officers were found violating</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>A city in peril - Newspaper - DAWN.COM</t>
+          <t>4 suspects involved in Lahore Underpass shooting incident arrested ...</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1874407</t>
+          <t>https://www.dawn.com/news/1897870</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>24-Nov-2024</t>
+          <t>14-Mar-2025</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>The Lahore we know today seems to be stifled by an unrelenting haze of pollution, neglect, and indifference. The city gasps for breath, choked by a thick</t>
+          <t>Lahore Police on Friday arrested four suspects allegedly involved in the Dharampura Underpass shooting incident, a video of which went viral a day ago.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Lahore goes for 'green lockdown' to tackle smog - Pakistan - DAWN ...</t>
+          <t>Overseas Pakistani woman attacked in Lahore's factory area: police ...</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868819</t>
+          <t>https://www.dawn.com/news/1905701</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>31-Oct-2024</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>The Punjab government imposed a “green lockdown” in designated smog hotspots across Lahore on Wednesday, imposing restrictions on barbecue joints, motorcycle-</t>
-        </is>
-      </c>
+          <t>21-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Lahore's urban disaster: From colonial sprawl to capitalist chaos ...</t>
+          <t>Five booked in 'rape' case of social media activist in Lahore ...</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1892744</t>
+          <t>https://www.dawn.com/news/1916345</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>17-Mar-2025</t>
+          <t>11-Jun-2025</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Requiem for a dying city - Lahore! Recommend 0. Dawn Logo Dawn News.</t>
+          <t>LAHORE: Police have registered a case against five people in connection with the alleged rape of a female social media activist. Reports</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Lahore receives highest rainfall of last 30 years: Wasa - Pakistan ...</t>
+          <t>After Rawalpindi, Lahore makes helmets mandatory for pillion riders ...</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1845401</t>
+          <t>https://www.dawn.com/news/1889425/after-rawalpindi-lahore-makes-helmets-mandatory-for-pillion-riders</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>12-Jul-2024</t>
+          <t>03-Feb-2025</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>While speaking to a private news channel today, Ghafran said that Wasa staff was actively engaged in drainage operations across the city, adding</t>
+          <t>اپنے آشیانوں کو مسمار ہوتے دیکھنا کیسا ہے؟ Dawn News English</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Worst air quality persists in Lahore with 708 AQI - Pakistan - DAWN ...</t>
+          <t>Three Mayo Hospital nurses removed over injection deaths in Lahore</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1868279</t>
+          <t>https://www.dawn.com/news/1897329</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>29-Oct-2024</t>
+          <t>12-Mar-2025</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lahore, yet again, topped the world map in the list of most polluted cities of the world. New Delhi followed it with AQI 232 at 11pm while its</t>
+          <t>LAHORE: The Punjab health department has initiated proceedings under the Punjab Employees Efficiency, Discipline and Accountability (Peeda)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English ...</t>
+          <t>Three Shalimar coaches derail at Shahdara bridge near Lahore ...</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909395</t>
+          <t>https://www.dawn.com/news/1888917</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>08-May-2025</t>
+          <t>01-Feb-2025</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>India-Pakistan Roundup | Blast In Lahore | Dawn News English.</t>
+          <t>Three passenger coaches of Shalimar Express derailed at Shahdara bridge, around 5-6km away from Lahore railway station, at 9am on Friday morning.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Suspect held for allegedly raping college student in Lahore: police ...</t>
+          <t>Boat tragedies prompt FIA to offload 2,500 in one month at Lahore ...</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1864994</t>
+          <t>https://www.dawn.com/news/1890925</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>13-Oct-2024</t>
+          <t>10-Feb-2025</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>A security guard who allegedly raped a student at a private college in Lahore has been arrested after news related to the incident went viral on social media.</t>
+          <t>“Lahore airport authorities are conducting rigorous screening of passengers under the directives of FIA Lahore chief Sarfraz Khan Virk. As</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Lahore police probing claims about disinformation that sparked UK ...</t>
+          <t>Lahore court cancels Nazish Jahangir's non-bailable arrest warrant ...</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1853208</t>
+          <t>https://images.dawn.com/news/1193411/lahore-court-cancels-nazish-jahangirs-non-bailable-arrest-warrant-after-she-attends-hearing</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>19-Aug-2024</t>
+          <t>22-Mar-2025</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Lahore Deputy Inspector General (Operations) Faisal Kamran told Dawn they were analysing the claims made by UK broadcaster ITV News and had</t>
+          <t>Latest Celebrity Culture Comment Local Her. DAWN · Latest · Celebrity · Culture ArtBooksFilm &amp; TVMusicNewsParentingRightsReviewsStyle</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Govt shuts primary schools in Lahore over record pollution ...</t>
+          <t>Two more bodies of Libya boat tragedy victims arrive in Lahore ...</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1869574</t>
+          <t>https://www.dawn.com/news/1908386</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>03-Nov-2024</t>
+          <t>04-May-2025</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>For days, Lahore's 14 million people has been enveloped by smog, a mix of fog and pollutants caused by low-grade diesel fumes, smoke from</t>
+          <t>Two more bodies of Pakistan nationals who lost their lives in a tragic boat accident off the eastern coast of Libya, arrived at Lahore Airport on Sunday.</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Parking chaos deepens in Lahore as agencies pass the buck - Dawn</t>
+          <t>Lahore police file case as YDA, hospital staff protest against 5-year ...</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1917362</t>
+          <t>https://www.dawn.com/news/1853579</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16-Jun-2025</t>
+          <t>21-Aug-2024</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>The city's civic authorities appear to have no workable solution for Lahore's worsening parking crisis, with plans for setback areas in front of buildings and</t>
+          <t>The staff of the Sir Ganga Ram Hospital (SGRH) and the Young Doctors Association (YDA) alleged that a five-year-old girl was raped on the facility's premises.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Poor vendor from Lahore falls victim to Indian drone - Pakistan - Dawn</t>
+          <t>Schools in Lahore and Multan divisions open today - Pakistan ...</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1909625</t>
+          <t>https://www.dawn.com/news/1873535</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>09-May-2025</t>
+          <t>20-Nov-2024</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Haider Ali, a vendor who was injured along with his two cousins when a drone crashed near Rawalpindi Cricket Stadium, succumbed to his injuries in the hospital</t>
+          <t>LAHORE: The Punjab government on Tuesday reopened schools in remaining divisions of Lahore and Multan from Wednesday (today) following an</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Leaders booked over pro-army rally in Lahore: PTI - Pakistan - Dawn</t>
+          <t>US envoy calls on Nawaz, Maryam in Lahore - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911521</t>
+          <t>https://www.dawn.com/news/1860735</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>17-May-2025</t>
+          <t>24-Sept-2024</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>LAHORE: The Pakistan Tehreek-i-Insaf (PTI) has claimed its leaders and workers have been booked for taking out a 'Pakistan Zindabad' rally,</t>
+          <t>LAHORE: US Ambassador to Pakistan Donald Blome called on PML-N President Nawaz Sharif and Chief Minister Maryam Nawaz here on Monday.</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19 die, 75 injured as windstorm, rain batter Punjab districts - Dawn</t>
+          <t>Fast-food chain outlet attacked in Lahore's DHA - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1913140</t>
+          <t>https://www.dawn.com/news/1903292</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>25-May-2025</t>
+          <t>10-Apr-2025</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>LAHORE: At least 19 people died while about 75 were injured as the heavy windstorm followed by rain battered various</t>
+          <t>LAHORE: An outlet of a fast-food chain on Wednesday came under an attack in Defense Housing Authority (DHA) when scores of people pelted it</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Fire at 220kV grid station in Lahore disrupts supply to several city ...</t>
+          <t>Torrential monsoon rains break 44-year-old record in Lahore ...</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1834687</t>
+          <t>https://www.dawn.com/news/1849386</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>01-Aug-2024</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>LAHORE: Almost half of the city plunged into darkness after the 220kV Sabzazar / Bund Road grid station caught fire causing a major</t>
+          <t>Torrential rains in Lahore broke a record of at least 44 years on Thursday as the city witnessed a maximum rainfall of almost 360 millimetres within hours in</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Escaped lion attacks woman and children in Lahore - Pakistan - Dawn</t>
+          <t>Lahore drug court directs urgent regulation of infant formula ...</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1922087/escaped-lion-attacks-woman-and-children-in-lahore</t>
+          <t>https://www.dawn.com/news/1909619</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>04-Jul-2025</t>
+          <t>09-May-2025</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>News and denials</t>
+          <t>LAHORE: In a landmark judgment, the Drug Court Lahore has directed authorities to take urgent steps to regulate the manufacturing, sale, and</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Art council, Ajoka theatre workshop from 16th - Newspaper - Dawn</t>
+          <t>Multiple casualties reported amid heavy rains across Punjab ...</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924314/art-council-ajoka-theatre-workshop-from-16th</t>
+          <t>https://www.dawn.com/news/1913072</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>24-May-2025</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>LAHORE: The Alhamra Arts Council, in collaboration with Ajoka Theatre, is going to launch the second annual edition</t>
+          <t>The data released by the PDMA showed that three people died in Lahore, two in Jhelum, one each in Rawalpindi, Sheikhupura, Nankana Sahib,</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News ...</t>
+          <t>Doctors, paramedics lock Lahore OPDs during protest - Pakistan ...</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1912424/pakistan-roundup-khuzdar-school-attack-india-blamed-pm-visits-quetta-dawn-news-english</t>
+          <t>https://www.dawn.com/news/1905844</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>21-May-2025</t>
+          <t>22-Apr-2025</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News English.</t>
+          <t>The young doctors and paramedics observed a strike at the outpatient departments (OPDs) of the government hospitals in Lahore and some other parts of Punjab.</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>PkMAP protests Afghans' repatriation in Quetta - Pakistan - Dawn</t>
+          <t>Lahore students demand transparent probe into 'rape, harassment ...</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1906860</t>
+          <t>https://www.dawn.com/news/1866742</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27-Apr-2025</t>
+          <t>22-Oct-2024</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Workers and supporters of the Pashtoonkhwa Milli Awami Party (PkMAP) took out a rally in support of Afghan refugees and urged the government of Pakistan to</t>
+          <t>The Student Action Committee Lahore, organised by students of various educational institutes, has called for transparent investigations into incidents of rape</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BNP-M demonstrators face tear gas, shelling amid sit-in near Quetta</t>
+          <t>Lahore woman 'gang-raped' in front of husband, child - Pakistan ...</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902476</t>
+          <t>https://www.dawn.com/news/1848007</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>06-Apr-2025</t>
+          <t>26-Jul-2024</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>The Balochistan National Party-Mengal (BNP-M) on Sunday evening announced that police used tear gas and shelling to disperse protesters during their sit-in.</t>
+          <t>LAHORE: A woman was allegedly gang-raped by robbers at gunpoint in front of her husband and a three-year-old daughter in Hafizabad district</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Two killed, 11 injured in explosion near Quetta: police - Dawn</t>
+          <t>Monetising hate - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914544</t>
+          <t>https://www.dawn.com/news/1866795</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>31-May-2025</t>
+          <t>22-Oct-2024</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>SHO identifies the deceased as Abdul Salam, owner of a coal mine, and his brother.</t>
+          <t>Regarding the alleged rape case in Lahore, news outlets and fact-checkers scrambled to provide context, even as the government and other</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>AKU concludes capacity building project with BAEC Quetta - Dawn</t>
+          <t>Cop shoots blasphemy suspect in Quetta lockup - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1920867/aku-concludes-capacity-building-project-with-baec-quetta</t>
+          <t>https://www.dawn.com/news/1858677</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>29-Jun-2025</t>
+          <t>13-Sept-2024</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Project brought together professionals to build institutional capacity in designing and conducting large-scale, sample-based assessments.</t>
+          <t>Police constable, who was posted at the Kharotabad station, arrested; IG says Sarhadi used his personal pistol.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Three cops among six injured in grenade attack in Quetta - Dawn</t>
+          <t>10, including FC soldier, injured in Quetta explosion: police ...</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915097</t>
+          <t>https://www.dawn.com/news/1894904</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>03-Jun-2025</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Officials say unidentified assailants attacked a police vehicle with a hand-grenade near Bakra Mandi at the Eastern Bypass area of the</t>
-        </is>
-      </c>
+          <t>28-Feb-2025</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1 dead, 10 injured in Quetta blast targeting convoy of PPP MPA Ali ...</t>
+          <t>Two killed, 11 injured in explosion near Quetta: police - Pakistan ...</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911023</t>
+          <t>https://www.dawn.com/news/1914544</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14-May-2025</t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Lawmaker remains unhurt; Balochistan CM, govt spokesperson and Bilawal call for action against culprits, denounce attack.</t>
+          <t>Two people were killed and 11 others were injured in an explosion in the Killi Mangal area near Quetta in Balochistan, a police official told Dawn.com on</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Tear gas, water cannon employed to disperse Baloch Yakjehti ...</t>
+          <t>Three cops among six injured in grenade attack in Quetta - Pakistan ...</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899479</t>
+          <t>https://www.dawn.com/news/1915097</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>22-Mar-2025</t>
+          <t>03-Jun-2025</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Mahrang Baloch claims 3 killed, 13 others injured; Balochistan govt spokesperson says police took action to open road.</t>
+          <t>QUETTA: Six people, including three policemen, were injured in a hand-grenade attack here on Monday. Officials said unidentified assailants</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Quetta braces for BNP long march as impasse persists - Dawn</t>
+          <t>3 dead, 21 injured in blast near police vehicle in Quetta market ...</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902347</t>
+          <t>https://www.dawn.com/news/1900656</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>06-Apr-2025</t>
+          <t>27-Mar-2025</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>BNP-M deadline for acceptance of its demands, including the release of Dr Mahrang Baloch, ended on Saturday midnight.</t>
+          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Quetta healthcare - Newspaper - DAWN.COM</t>
+          <t>Quetta braces for BNP long march as impasse persists - Pakistan ...</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1890571</t>
+          <t>https://www.dawn.com/news/1902347</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>08-Feb-2025</t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>QUETTA, known for its changing weather patterns, often sees a surge in the number of patients requiring medical</t>
+          <t>BNP-M deadline for acceptance of its demands, including the release of Dr Mahrang Baloch, ended on Saturday midnight.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>One killed, four injured in Quetta car blast - Pakistan - DAWN.COM</t>
+          <t>BNP-M demonstrators face tear gas, shelling amid sit-in near Quetta ...</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914838</t>
+          <t>https://www.dawn.com/news/1902476</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>02-Jun-2025</t>
+          <t>06-Apr-2025</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Police say it was a targeted attack, in which a magnetic bomb was detonated remotely; responsibility not accepted by any group.</t>
+          <t>Party chief Sardar Akhtar Mengal faces arrest if his party enters Quetta, Balochistan govt warns.</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Quetta, 1935: Empire, earthquake, and the limits of control - Dawn</t>
+          <t>Two cops martyred in Quetta attack - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914296</t>
+          <t>https://www.dawn.com/news/1893257</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>31-May-2025</t>
+          <t>21-Feb-2025</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Research on the 1935 Quetta earthquake is shockingly limited, where anthropologists and historians can study colonial policies and</t>
+          <t>QUETTA: Two police personnel were martyred and four armed attackers were killed in a heavy gun battle during an attack on a police post in</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Gun, bomb attacks claim three lives in Dera, Quetta - Pakistan - Dawn</t>
+          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914636</t>
+          <t>https://www.dawn.com/news/1897237</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>01-Jun-2025</t>
+          <t>11-Mar-2025</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>A Levies official was martyred in a shooting in Dera Bugti and a Levies police station was set on fire in Mastung district, while a roadside blast on the</t>
+          <t>The reports said that security forces had surrounded the area and launched a clearance operation to rescue all passengers. The Mashkaf Tunnel is</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>BNP-M reaches Kalat in march to Quetta against crackdown ... - Dawn</t>
+          <t>Govt keeps BNP-M long march to Quetta at bay - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900877</t>
+          <t>https://www.dawn.com/news/1902575</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>28-Mar-2025</t>
+          <t>07-Apr-2025</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>The BNP-M had announced a long march from Wadh to Quetta today to protest against the arrests of Baloch Yakjehti Committee (BYC) leaders and activists.</t>
+          <t>Law enforcement personnel encircle sit-in to arrest Mengal; party calls for strike across Balochistan today.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Indian boycott of Turkish goods condemned in Quetta - Dawn</t>
+          <t>President Zardari urges need to win 'war against terrorism' during ...</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1911468</t>
+          <t>https://www.dawn.com/news/1898968</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>17-May-2025</t>
+          <t>19-Mar-2025</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Traders say Pakistan aspires to have good trade relations with all countries.</t>
+          <t>President Asif Ali Zardari on Wednesday emphasised the need to win the “war against terrorism” at all costs during a visit to Quetta.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Govt employees violently clash with police in Quetta - Pakistan - Dawn</t>
+          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits ...</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1919872</t>
+          <t>https://www.dawn.com/news/1912424/pakistan-roundup-khuzdar-school-attack-india-blamed-pm-visits-quetta-dawn-news-english</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>25-Jun-2025</t>
+          <t>21-May-2025</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>QUETTA: Police arrested over two dozen government employees' on Tuesday after clashes erupted while they were protesting against their</t>
+          <t>Pakistan Roundup: Khuzdar School Attack, India Blamed, PM Visits Quetta | Dawn News English.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>HBL PSL 2025: Abrar tears through Peshawar Zalmi batting ... - Dawn</t>
+          <t>Quetta transport - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903765</t>
+          <t>https://www.dawn.com/news/1840041</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>12-Apr-2025</t>
+          <t>15-Jun-2024</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>The mystery spinner gets 4 wickets as Peshawar get bundled out for 136 in their first outing; Quetta top-order fires to set up massive win.</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>26 martyred in Quetta railway station explosion - Pakistan - Dawn</t>
+          <t>Doctor among three killed in Quetta blast - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1871371</t>
+          <t>https://www.dawn.com/news/1900758</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10-Nov-2024</t>
+          <t>28-Mar-2025</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>At least 26 people, including 16 security personnel, lost their lives and 61 others were injured in a suicide bombing at a Quetta railway station on Saturday.</t>
+          <t>QUETTA: At least three people, including a leading oncologist, were killed and 21 injured in a bomb blast on a major road of the provincial</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Hindus in Quetta protest Indian accusations over Pahalgam attack</t>
+          <t>BNP-M reaches Kalat in march to Quetta against crackdown on ...</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1907649</t>
+          <t>https://www.dawn.com/news/1900877</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>01-May-2025</t>
+          <t>28-Mar-2025</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Members of the Hindu community staged a protest rally in Quetta on Wednesday, condemning what they called baseless allegations against Pakistan by the Indian</t>
+          <t>The BNP-M had announced a long march from Wadh to Quetta today to protest against the arrests of Baloch Yakjehti Committee (BYC) leaders and activists.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>3 dead, 21 injured in blast near police vehicle in Quetta market - Dawn</t>
+          <t>AKU concludes capacity building project with BAEC Quetta ...</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900656</t>
+          <t>https://www.dawn.com/news/1920867/aku-concludes-capacity-building-project-with-baec-quetta</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>27-Mar-2025</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Three people were killed and 21 others injured after an explosion occurred near a police vehicle in the Barech Market area on Quetta's Double Road, officials</t>
-        </is>
-      </c>
+          <t>29-Jun-2025</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Unprivileged to get legal aid at state expense - Pakistan - DAWN.COM</t>
+          <t>Quetta bombing - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924282</t>
+          <t>https://www.dawn.com/news/1871374</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>10-Nov-2024</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Initiative to be implemented across all levels of the judiciary, from magistrate courts to the Supreme Court.</t>
+          <t>THERE appears to be no end to the stream of violent incidents occurring in Balochistan, indicating a clear failure</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Gas explosion claims two lives in Quetta - Pakistan - DAWN.COM</t>
+          <t>Relatives not allowed to meet, deliver food to Mahrang Baloch in ...</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1896528</t>
+          <t>https://www.dawn.com/news/1899848</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>08-Mar-2025</t>
+          <t>23-Mar-2025</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>A young girl and her mother were killed, while a minor boy was injured in an explosion inside a house near the Hazar Gangi area on the outskirts of the</t>
+          <t>Relatives are not being allowed to meet and deliver food to Dr Mahrang Baloch while she is in custody in Quetta District Jail, the Baloch Yakjehti Committee (</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Four Frontier Corps personnel martyred, three injured in Quetta ...</t>
+          <t>Gun, bomb attacks claim three lives in Dera, Quetta - Pakistan ...</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1906502</t>
+          <t>https://www.dawn.com/news/1914636</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>25-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Four Frontier Corps (FC) personnel were martyred and three other suffered injuries in an explosion near a security vehicle in Quetta's Margate area, police</t>
-        </is>
-      </c>
+          <t>01-Jun-2025</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>President Zardari urges need to win 'war against terrorism' during ...</t>
+          <t>Death toll rises to 26 in Quetta Railway Station blast, 62 injured ...</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1898968</t>
+          <t>https://www.dawn.com/news/1871234</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>19-Mar-2025</t>
+          <t>09-Nov-2024</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>President Asif Ali Zardari on Wednesday emphasised the need to win the “war against terrorism” at all costs during a visit to Quetta.</t>
+          <t>Speaking to Geo News, he said that besides civilians, “some law enforcement” personnel were also martyred. According to Reuters, Balochistan</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Protesters take away bodies from Quetta hospital morgue - Dawn</t>
+          <t>Quetta's Achakzai Colony hit by rocket attack - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899300</t>
+          <t>https://www.dawn.com/news/1867254</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>21-Mar-2025</t>
+          <t>24-Oct-2024</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Authorities claim corpses belonged to Jaffar Express attackers; BYC activists say families had been protesting for days to see bodies.</t>
+          <t>QUETTA / KHUZDAR: Rockets hit the wall of Achakzai residential colony on Quetta's Khojak Road, while two men were injured in a grenade</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
+          <t>Quetta police official allegedly kills blasphemy suspect in jail ...</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914774</t>
+          <t>https://www.dawn.com/news/1858556</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>01-Jun-2025</t>
+          <t>12-Sept-2024</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
+          <t>A Quetta police officer allegedly killed a man being held in custody on suspicion of blasphemy charges, police officials said on Thursday.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Rescue operation for hostages underway after terrorists attack Jaffar ...</t>
+          <t>Four Frontier Corps personnel martyred, three injured in Quetta ...</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897237</t>
+          <t>https://www.dawn.com/news/1906502</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>11-Mar-2025</t>
+          <t>25-Apr-2025</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Radio Pakistan, late Tuesday night, reports 13 terrorists killed, 80 hostages rescued; first relief train carrying passengers reaches Mach;</t>
+          <t>Four Frontier Corps (FC) personnel were martyred and three other suffered injuries in an explosion near a security vehicle in Quetta's Margate area, police</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>PIA to resume direct flights from Quetta to Jeddah - Pakistan - Dawn</t>
+          <t>Quetta, 1935: Empire, earthquake, and the limits of control - Pakistan ...</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1846448</t>
+          <t>https://www.dawn.com/news/1914296</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>18-Jul-2024</t>
+          <t>31-May-2025</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Pakistan International Airlines (PIA) on Thursday announced that it will resume direct flights from Quetta to the Saudi Arabian capital of Jeddah from next</t>
+          <t>As we also see in the June 3 news report, the British Raj had quoted 20,000 people dead with 10,000 survivors — later government reports would</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>COAS Munir vows to 'crush Indian-sponsored terrorists' with support ...</t>
+          <t>BNP supporters block Quetta-Karachi National Highway - Pakistan ...</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914774</t>
+          <t>https://www.dawn.com/news/1896255</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>01-Jun-2025</t>
+          <t>07-Mar-2025</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir has vowed to “crush” terrorists in Balochistan, stating that India's involvement in terrorism in the</t>
+          <t>Hundreds of workers and supporters of the Balochistan National Party-Mengal blocked the Quetta-Karachi National Highway at Wadh, near Khuzdar, on Thursday in</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Footprints: GRIEF, ANGER RULE QUETTA STATION - Dawn</t>
+          <t>BNP-M long march against arrests leaves Mastung for Quetta ...</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1871777</t>
+          <t>https://www.dawn.com/news/1901009</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>12-Nov-2024</t>
+          <t>29-Mar-2025</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>A sombre mood prevails over the grandiose Quetta Railway Station. The whiff of carnage that took place here two days ago is palpable in the air.</t>
+          <t>QUETTA/ KHUZDAR: The long march, launched by the Balochistan National Party (BNP-Mengal) to protest the arrest of BYC chief organiser Dr</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
+          <t>On Quetta visit, PM Shehbaz says Balochistan attacks 'wicked ...</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901943</t>
+          <t>https://www.dawn.com/news/1855483</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>04-Apr-2025</t>
+          <t>29-Aug-2024</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -2532,990 +2528,956 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>BNP supporters block Quetta-Karachi National Highway - Dawn</t>
+          <t>Quetta records 65 acts of terrorism in 2024 - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1896255</t>
+          <t>https://www.dawn.com/news/1881746</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>07-Mar-2025</t>
+          <t>29-Dec-2024</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Hundreds of workers and supporters of the Balochistan National Party-Mengal blocked the Quetta-Karachi National Highway at Wadh, near Khuzdar, on Thursday in</t>
+          <t>QUETTA: As many as 365 people, including security personnel, have been martyred and several injured in terrorist attacks, targeted killings,</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>One hurt in grenade attack on Quetta police station - Pakistan - Dawn</t>
+          <t>Hindus in Quetta protest Indian accusations over Pahalgam attack ...</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1904124</t>
+          <t>https://www.dawn.com/news/1907649</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>14-Apr-2025</t>
+          <t>01-May-2025</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Police say unidentified motorcyclist hurled grenade at Kachi Baig police station, which exploded near the gate.</t>
+          <t>Members of the Hindu community staged a protest rally in Quetta on Wednesday, condemning what they called baseless allegations against Pakistan by the Indian</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Balochistan govt warns BNP-M to limit march to Quetta's Sariab ...</t>
+          <t>1 dead, 10 injured in Quetta blast targeting convoy of PPP MPA Ali ...</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902266</t>
+          <t>https://www.dawn.com/news/1911023</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>05-Apr-2025</t>
+          <t>14-May-2025</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Balochistan government spokesperson Shahid Rind on Saturday offered the Balochistan National Party-Mengal (BNP-M) to march till Quetta's Shahwani Stadium on</t>
+          <t>One person was killed and 10 others injured when a blast struck the convoy of PPP MPA Ali Madad Jattak in Quetta on Wednesday, but the lawmaker was unharmed.</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Two Balochistan highways open for traffic after a week - Dawn</t>
+          <t>BNP leader killed, cousin injured in Quetta shooting - Pakistan ...</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1897163</t>
+          <t>https://www.dawn.com/news/1861833</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11-Mar-2025</t>
+          <t>29-Sept-2024</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Traffic on Quetta-Karachi RCD Highway, Quetta-Taftan Highway (in Mastung), Karachi-Panjgur Highway, and Quetta-Sibi Highway had been blocked</t>
+          <t>A senior leader of the Balochistan National Party-Mengal (BNP-M), Agha Khalid Shah, was shot dead by unidentified assailants in Quetta on Saturday.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Quetta-Sibi road reopened after gun battle in Bolan - Pakistan - Dawn</t>
+          <t>CM Bugti takes notice of fire in 'historical' Quetta college - Pakistan ...</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1893896</t>
+          <t>https://www.dawn.com/news/1856561</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>24-Feb-2025</t>
+          <t>03-Sept-2024</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Three militants were killed in an hour-long exchange of fire between security forces and two armed groups which had blocked the Quetta-Sibi highway.</t>
+          <t>QUETTA: The Balochistan chief minister and education minister have taken notice of the fire that gutted the building of Postgraduate</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Strike observed in many areas of Balochistan on BNP-M call - Dawn</t>
+          <t>PkMAP protests Afghans' repatriation in Quetta - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902827</t>
+          <t>https://www.dawn.com/news/1906860</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>08-Apr-2025</t>
+          <t>27-Apr-2025</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Party leader claims 4 workers injured by police; 70 picked up and 4 jailed.</t>
+          <t>QUETTA: Workers and supporters of the Pashtoonkhwa Milli Awami Party (PkMAP) took out a rally in support of Afghan refugees and urged the</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Poet shot dead in Quetta - Pakistan - DAWN.COM</t>
+          <t>9, including 3 children, injured in Quetta blast - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908757</t>
+          <t>https://www.dawn.com/news/1806546</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>06-May-2025</t>
+          <t>17-Jan-2024</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Mir Allah Bakhsh Shahzad, a local Brahvi language poet and writer, was shot dead by unknown armed men in Sabzal Road area of the provincial capital on Monday.</t>
+          <t>Nine people, including a traffic policeman and three children, were injured in a blast on Quetta's Zarghoon Road on Wednesday, according to</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ECP announces schedule for Quetta local bodies' polls - Dawn</t>
+          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1915718</t>
+          <t>https://www.dawn.com/news/1901075</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>06-Jun-2025</t>
+          <t>29-Mar-2025</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Returning officers will issue public notices on June 23; candidates can submit nomination papers between June 24 and 27.</t>
+          <t>However, the Quetta administration has denied the BNP-M permission to go ahead with its rally. Marchers and motorists from different political</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>BHC to hear pleas against mines law on 21st - Pakistan - DAWN.COM</t>
+          <t>Gas explosion claims two lives in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924274/bhc-to-hear-pleas-against-mines-law-on-21st</t>
+          <t>https://www.dawn.com/news/1896528</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>08-Mar-2025</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Petitions filed by JUI-F, PkMAP, BNP-Mengal, National Party, Nawabzada Lashkri Raisani and Mir Humayun Kurd.</t>
+          <t>QUETTA: A young girl and her mother were killed, while a minor boy was injured in an explosion inside a house near the Hazar Gangi area on</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Quetta transport - Newspaper - DAWN.COM</t>
+          <t>Jaffar Express operation complete, 33 terrorists killed: DG ISPR ...</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1840041</t>
+          <t>https://www.dawn.com/news/1897419</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15-Jun-2024</t>
+          <t>12-Mar-2025</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>SECTIONS of the press have reported that the federal government is not agreeable to allocating funds for the procurement of 100 buses for</t>
+          <t>According to railway officials, the train had 440 passengers,” he said while speaking in an interview on Dunya News show 'On the Front'. The</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
+          <t>Footprints: GRIEF, ANGER RULE QUETTA STATION - Newspaper ...</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901075</t>
+          <t>https://www.dawn.com/news/1871777</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>29-Mar-2025</t>
+          <t>12-Nov-2024</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
+          <t>A sombre mood prevails over the grandiose Quetta Railway Station. The whiff of carnage that took place here two days ago is palpable in the air.</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Quetta records 65 acts of terrorism in 2024 - Pakistan - DAWN.COM</t>
+          <t>Balochistan govt warns BNP-M to limit march to Quetta's Sariab ...</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1881746</t>
+          <t>https://www.dawn.com/news/1902266</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>29-Dec-2024</t>
+          <t>05-Apr-2025</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>QUETTA: As many as 365 people, including security personnel, have been martyred and several injured in terrorist attacks, targeted killings,</t>
+          <t>Balochistan government spokesperson Shahid Rind on Saturday offered the Balochistan National Party-Mengal (BNP-M) to march till Quetta's Shahwani Stadium on</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>'RDMC committed to empowering people through employment ...</t>
+          <t>Complete shutdown in Quetta over student's kidnapping - Pakistan ...</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924276</t>
+          <t>https://www.dawn.com/news/1873571</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>20-Nov-2024</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>QUETTA: Barrick Mining Corporation CEO Mark Bristow has reaffirmed Reko Diq Mining Company's (RDMC) commitment to empowering the people of</t>
+          <t>QUETTA: A complete shutdown was observed in the provincial capital on Tuesday in protest against the kidnapping of an 11-year-old student,</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Three killed, nine injured in road accidents - Newspaper - DAWN.COM</t>
+          <t>Cellphone, internet services in Quetta suspended till Ashura ...</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1924281/three-killed-nine-injured-in-road-accidents</t>
+          <t>https://www.dawn.com/news/1845820</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>15-Jul-2024</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>A pickup truck carrying a wedding party overturned near Chaman toll plaza, killing three people and injuring seven others, according to Levies</t>
+          <t>Balochistan govt says over 18000 security personnel will be deployed in Quetta on Youm-i-Ashur.</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Akhtar Mengal, others remain unhurt after suicide blast near rally on ...</t>
+          <t>Seven injured in Quetta grenade attack - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901075</t>
+          <t>https://www.dawn.com/news/1842404</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>29-Mar-2025</t>
+          <t>28-Jun-2024</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Sardar Akhtar Mengal and other workers of his faction of the Balochistan National Party (BNP-M) remained unhurt on Saturday after a suicide bomber blew himself</t>
+          <t>QUETTA: Seven people were injured when some unidentified motorcyclists lobbed a hand grenade at a vehicle carrying members of security</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Over 400 cameras installed in Quetta - Pakistan - DAWN.COM</t>
+          <t>10 picnickers kidnapped from Quetta outskirts - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1806194</t>
+          <t>https://www.dawn.com/news/1840951</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16-Jan-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>QUETTA: More than 400 IP cameras have been installed at around 225 locations as part of the Quetta Safe City Project, officials working on</t>
+          <t>QUETTA: Unknown armed men kidnapped at least 10 people, including a customs officer, from Shaban, a picnic point on the outskirts of the</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Armed men torch several govt buildings in Kalat - Pakistan - Dawn</t>
+          <t>PM Shehbaz calls for national unity, dialogue against terrorism after ...</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908061</t>
+          <t>https://www.dawn.com/news/1897669</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>03-May-2025</t>
+          <t>13-Mar-2025</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Unknown armed men blocked the Quetta-Karachi Highway in the Mongochar area of Kalat district and set fire to several government buildings in the Mongochar</t>
+          <t>Prime Minister Shehbaz Sharif speaks in Quetta on Thursday. — DawnNewsTV.</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Relatives not allowed to meet, deliver food to Mahrang Baloch in ...</t>
+          <t>Man gunned down in Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1899848</t>
+          <t>https://www.dawn.com/news/1890268</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>23-Mar-2025</t>
+          <t>07-Feb-2025</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Relatives are not being allowed to meet and deliver food to Dr Mahrang Baloch while she is in custody in Quetta District Jail, the Baloch Yakjehti Committee (</t>
+          <t>QUETTA: Unknown armed assailants opened fire and killed a man in the provincial capital on Thursday. Police said motorcyclists opened fire</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>PSL 10 trophy unveiled in Quetta amid fanfare - Pakistan - Dawn</t>
+          <t>Mengal warns of march on Quetta - Newspaper - DAWN.COM</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902576</t>
+          <t>https://www.dawn.com/news/1901943</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>07-Apr-2025</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Unveiling ceremony attended by international cricketer from the province Haseebullah Khan.</t>
-        </is>
-      </c>
+          <t>04-Apr-2025</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Woman dies of Congo fever in Quetta - Pakistan - DAWN.COM</t>
+          <t>7 dead, 19 injured in Quetta bus accident: officials - DAWN.COM</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1858850</t>
+          <t>https://www.dawn.com/news/1862839</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>14-Sept-2024</t>
+          <t>03-Oct-2024</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>The patient was brought from Musakhail district in critical condition with suspected Congo virus and admitted to the Fatima Jinnah Chest</t>
+          <t>Seven people were killed and 19 people were injured when a bus fell into a ravine near Quetta's Brewery Roads Bypass area on Thursday, according to officials.</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Snowfall in Balochistan disrupts traffic - Pakistan - DAWN.COM</t>
+          <t>HBL PSL 2025: Abrar tears through Peshawar Zalmi batting lineup ...</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1886462</t>
+          <t>https://www.dawn.com/news/1903765</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>20-Jan-2025</t>
+          <t>12-Apr-2025</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Heavy rain and snowfall disrupted transportation across several towns and cities in Balochistan, while residents of Quetta faced severe hardships.</t>
+          <t>The mystery spinner gets 4 wickets as Peshawar get bundled out for 136 in their first outing; Quetta top-order fires to set up massive win.</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Drinking water supply in Quetta restored - Pakistan - DAWN.COM</t>
+          <t>Cop martyred, 6 injured in blast near ATF vehicle in Quetta: police ...</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901936</t>
+          <t>https://www.dawn.com/news/1898108</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>04-Apr-2025</t>
+          <t>15-Mar-2025</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Official says water filtration plants in Duki, Pishin, Loralai and Kachhi to become fully operational by April 30.</t>
+          <t>A cop was martyred while six others were wounded in a blast near a vehicle of Balochistan's Anti-Terrorist Force (ATF) in Quetta on Saturday, according to</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>New polio case found in Quetta, taking this year's tally to 33 - Dawn</t>
+          <t>28 dead, 22 injured as Quetta-bound bus falls into ravine in ...</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865282</t>
+          <t>https://www.dawn.com/news/1836392</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15-Oct-2024</t>
+          <t>29-May-2024</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>According to an official of the Regional Reference Laboratory for Polio Eradication at the National Institute of Health Islamabad, the wild</t>
+          <t>However, AC Mengal said that rescue officials reached the location as soon as they received the news. According to the AC, most of the deceased</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Field Marshal Asim Munir assails India's 'hydro-terrorism ... - Dawn</t>
+          <t>14 injured as PTI workers, police clash in Quetta - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914324</t>
+          <t>https://www.dawn.com/news/1871205</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>30-May-2025</t>
+          <t>09-Nov-2024</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Chief of Army Staff (COAS) Field Marshal Asim Munir on Friday emphasised the need for a peaceful resolution to the Kashmir dispute, assailing India's “unlawful</t>
+          <t>QUETTA: Fourteen people, including eight cops, were injured when clashes erupted between the police and PTI supporters on Friday after the</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Two killed, six injured as vehicle plunges into ravine along Quetta ...</t>
+          <t>Cop among 12 injured in Quetta blast targeting police van - Pakistan ...</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1857621</t>
+          <t>https://www.dawn.com/news/1861050</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>08-Sept-2024</t>
+          <t>25-Sept-2024</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Officials say Inspector Jumma Khan of the Mineral Department was travelling to Zhob with his family when the vehicle veered off a narrow</t>
+          <t>Twelve people were injured in a blast that targeted a police van near Eastern Bypass in Quetta, hospital and government officials said on Wednesday.</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Journalists in Balochistan decry job cuts, censorship - Pakistan - Dawn</t>
+          <t>Protesters take away bodies from Quetta hospital morgue - Pakistan ...</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908335</t>
+          <t>https://www.dawn.com/news/1899300</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>04-May-2025</t>
+          <t>21-Mar-2025</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>The journalist community in Balochistan has called on the government to take urgent steps to ensure their safety, uphold press freedom, address widespread</t>
+          <t>QUETTA: Relatives of missing persons, who had been demanding they be allowed to identify dead bodies brought to the Civil Hospital,</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Plan finalised to increase Quetta Metropolitan Corporation's revenue</t>
+          <t>Two Balochistan highways open for traffic after a week - Pakistan ...</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1875870</t>
+          <t>https://www.dawn.com/news/1897163</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>01-Dec-2024</t>
+          <t>11-Mar-2025</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>QUETTA: Quetta Metropolitan Corporation (QMC) Administrator Muhammad Hamza Shafqaat has said a a strategy has been finalised to increase QMC</t>
+          <t>Traffic on Quetta-Karachi RCD Highway, Quetta-Taftan Highway (in Mastung), Karachi-Panjgur Highway, and Quetta-Sibi Highway had been blocked</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Night travel banned on key highways in Balochistan - Pakistan - Dawn</t>
+          <t>11 dead from gas leak in coal mine near Quetta - DAWN.COM</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1901307</t>
+          <t>https://www.dawn.com/news/1837542</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>30-Mar-2025</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>DC orders bar mostly public transport on arteries connecting Karachi, Sukkur, DI Khan, Multan to Quetta, Gwadar, and other cities.</t>
-        </is>
-      </c>
+          <t>03-Jun-2024</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>At Balochistan grand jirga, PM stresses need to win back 'misled ...</t>
+          <t>Marchers protesting Iran border closure reach Quetta - Pakistan ...</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1914525</t>
+          <t>https://www.dawn.com/news/1837027</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>31-May-2025</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Prime Minister Shehbaz Sharif on Saturday said that people who were “misled” by terrorists in Balochistan must be brought back on board.</t>
+          <t>Protest leader says they will not call off their protest in Quetta until the opening of the crossing point.</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Three martyred in attack on police van in Quetta - Pakistan - Dawn</t>
+          <t>One hurt in grenade attack on Quetta police station - Pakistan ...</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1903242</t>
+          <t>https://www.dawn.com/news/1904124</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10-Apr-2025</t>
+          <t>14-Apr-2025</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab area late on Wednesday night.</t>
+          <t>A passer-by was injured in the blast and was immediately shifted to Civil Hospital Quetta for treatment. The explosion damaged the police</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>PAC miffed at delay in street lights installation in Quetta - Dawn</t>
+          <t>2 injured in grenade attack on Quetta security checkpoint: police ...</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865482</t>
+          <t>https://www.dawn.com/news/1856189</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16-Oct-2024</t>
+          <t>01-Sept-2024</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>QUETTA: The Public Accounts Committee of the Balochistan Assembly, while discussing financial affairs of the local</t>
+          <t>Two bystanders were injured on Sunday in a grenade attack on a security checkpoint in Quetta's Chaman Phatak area, according to a senior police official.</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In ... - Dawn</t>
+          <t>One killed, four injured in Quetta car blast - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1900685</t>
+          <t>https://www.dawn.com/news/1914838</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>27-Mar-2025</t>
+          <t>02-Jun-2025</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Top News: 3 Dead, 21 Injured In Blast Near Police Vehicle In Quetta Market | Dawn News English.</t>
+          <t>QUETTA: One person was killed and four others injured — one of them seriously — in a bomb explosion in a vehicle in the provincial capital</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Govt keeps BNP-M long march to Quetta at bay - Pakistan - Dawn</t>
+          <t>Govt employees violently clash with police in Quetta - Pakistan ...</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1902575</t>
+          <t>https://www.dawn.com/news/1919872/govt-employees-violently-clash-with-police-in-quetta</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>07-Apr-2025</t>
+          <t>25-Jun-2025</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Law enforcement personnel encircle sit-in to arrest Mengal; party calls for strike across Balochistan today.</t>
+          <t>QUETTA: Police arrested over two dozen government employees' on Tuesday after clashes erupted while they were protesting against their</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Journalists to observe black day today against Quetta incident - Dawn</t>
+          <t>Quetta police station attacked amid protest against 'blasphemy ...</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1834744</t>
+          <t>https://www.dawn.com/news/1858440</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>12-Sept-2024</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>KARACHI: Different factions of the Pakistan Federal Union of Journalists (PFUJ) and Karachi Union of Journalists</t>
+          <t>QUETTA: The Kharotabad police station came under a grenade attack during a violent protest on Wednesday as an enraged mob demanded that the</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>HBL PSL 2025: Quetta Gladiators upstage Islamabad United ... - Dawn</t>
+          <t>ECP reschedules polls in Sibi, Quetta - Pakistan - DAWN.COM</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1908302</t>
+          <t>https://www.dawn.com/news/1872067</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>04-May-2025</t>
+          <t>13-Nov-2024</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>LAHORE: Lady luck was smiling brightly on young Hasan Nawaz here at the Gaddafi Stadium Saturday night. It was a genuine thriller as in-form</t>
+          <t>By-election in Sibi's PB-8 to now be on Nov 17, while re-polling in Quetta's PB-44 to be on Dec 12.</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Short circuit blamed for Quetta college blaze - Pakistan - DAWN.COM</t>
+          <t>Panjgur DC killed in attack on Quetta-Karachi highway - Pakistan ...</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1859465</t>
+          <t>https://www.dawn.com/news/1851938</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>17-Sept-2024</t>
+          <t>13-Aug-2024</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Speaking at a joint press conference, Mr Mandokhail, Deputy Commissioner Quetta Saad bin Asad and Principal of Science College Mohammad Azmat</t>
+          <t>News and denials</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Cop martyred, 6 injured in blast near ATF vehicle in Quetta: police</t>
+          <t>3 of 10 picnickers abducted from Quetta return home - Pakistan ...</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1898108</t>
+          <t>https://www.dawn.com/news/1841885</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>15-Mar-2025</t>
+          <t>25-Jun-2024</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Vehicle belongs to Anti-Terrorist Force; three of the personnel seriously injured, says medical superintendent at Bolan Medical Complex.</t>
+          <t>Three of the 10 men abducted last week by unknown armed men from Shaban — a picnic point on the outskirts of Quetta — returned home on</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Rally staged in Quetta for recovery of kidnapped tribesmen - Dawn</t>
+          <t>Cop martyred in Quetta by unidentified gunmen: police - Pakistan ...</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1865038</t>
+          <t>https://www.dawn.com/news/1888658</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14-Oct-2024</t>
+          <t>30-Jan-2025</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>QUETTA: Members of the Bugti Rabita Committee staged a demonstration on Sunday against the bandits of kacha area of Sindh, demanding</t>
+          <t>A policeman was martyred in Quetta when unidentified assailants shot him dead in the early hours of Thursday as he was returning home from work.</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Missing persons' camp burnt down in Quetta - Pakistan - DAWN.COM</t>
+          <t>Traffic jam in Quetta after kidnapping of tribal elder's son - Pakistan ...</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1870633</t>
+          <t>https://www.dawn.com/news/1872685</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>07-Nov-2024</t>
+          <t>16-Nov-2024</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Unidentified individuals set fire to the main camp of the Voice for Baloch Missing Persons (VBMP) near Quetta Press Club on Wednesday.</t>
+          <t>The protest was called off late at night after negotiations between the protesters and the Quetta deputy inspector general of police. The DIG</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Methane explosion traps 12 inside coal mine near Quetta - Dawn</t>
+          <t>World leaders condemn suicide bombing at Quetta railway station ...</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1884221</t>
+          <t>https://www.dawn.com/news/1871365</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>10-Jan-2025</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>QUETTA: At least 12 coal miners were trapped inside a mine after an explosion caused by methane gas in the Sanjdi coal field area, around 40</t>
-        </is>
-      </c>
+          <t>10-Nov-2024</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>4 bodies recovered, search continues for 8 others after mine ... - Dawn</t>
+          <t>Three martyred in attack on police van in Quetta - Pakistan - DAWN ...</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1884307</t>
+          <t>https://www.dawn.com/news/1903242</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>10-Jan-2025</t>
+          <t>10-Apr-2025</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>The bodies of four miners were recovered on Friday during a rescue operation near a coal mine in Quetta after a dozen mineworkers were left trapped therein.</t>
+          <t>QUETTA: Three personnel, including a police inspector, were martyred and another injured in an ambush at a police mobile van in the Sariab</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Complete shutdown in Quetta over student's kidnapping - Dawn</t>
+          <t>Bail plea of Quetta cop who killed blasphemy suspect filed ...</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1873571</t>
+          <t>https://www.dawn.com/news/1860158</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>20-Nov-2024</t>
+          <t>21-Sept-2024</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>A complete shutdown was observed in the provincial capital on Tuesday in protest against the kidnapping of an 11-year-old student.</t>
+          <t>Saad Khan Sarhadi's application filed in a local court after his family handed over case to Quetta Bar Association president.</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Centre rejects 100 green buses plan for Quetta - Pakistan - Dawn</t>
+          <t>Quetta Metropolitan Corporation fires 1,400 'ghost' employees ...</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1838091</t>
+          <t>https://www.dawn.com/news/1852998</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>06-Jun-2024</t>
+          <t>18-Aug-2024</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Balochistan is the only province that has no mass transit transport facility.</t>
+          <t>Mr Shafqaat, who is also the Quetta division commissioner, stated that most of the dismissed employees belonged to sanitation, fire brigade and</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>The killer highways of Balochistan - Pakistan - DAWN.COM</t>
+          <t>Race to rescue Jaffar Express hostages in Balochistan - Newspaper ...</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://www.dawn.com/news/1895508</t>
+          <t>https://www.dawn.com/news/1897307</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>05-Mar-2025</t>
+          <t>12-Mar-2025</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>“Is the road safe?” Muhammad Ahmed, who was travelling from Quetta to Dera Ismail Khan after 15 long years, asked the bus driver. News over</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Protests persist in Balochistan against alleged rigging - Dawn</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>https://www.dawn.com/news/1814552</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>16-Feb-2024</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>QUETTA: Supporters of</t>
+          <t>QUETTA: An unprecedented hostage situation unfolded on Tuesday after terrorists attacked the Jaffar Express in a rugged part of Balochistan</t>
         </is>
       </c>
     </row>

</xml_diff>